<commit_message>
Added Notes to SpecialOffer Excel Demos
</commit_message>
<xml_diff>
--- a/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
+++ b/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="156">
   <si>
     <t>ItemType</t>
   </si>
@@ -483,6 +483,42 @@
   </si>
   <si>
     <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Hier wäre folgende Konstellation denkbar: 8 (4,4) und 8 (4,4), aber die Regel ist, immer die grösste Anzahl Days zuerst auszuprobieren, und dass sind die 14 Days mit dem DayString 7,7. Daher hat dieser eine höhere Gewichtung und die gleichen Regeln kommen zu tragen wie beim Duration=15 . Es sind noch zwei Tage übrig, aber es sind keine Regeln mehr vorhanden mit dem Anfangstag 25JAN mit Days &lt;= 2, also wird die Berechnung abgebrochen.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Hier wäre folgende Konstellation denkbar: 8 (4,4) und 8 (4,4), aber die Regel ist, immer die grösste Anzahl Days zuerst auszuprobieren, und dass sind die 14 Days mit dem DayString 7,7. Daher hat dieser eine höhere Gewichtung und die gleichen Regeln kommen zu tragen wie beim Duration=15 . Es sind noch drei Tage übrig, aber es sind keine Regeln mehr vorhanden mit dem Anfangstag 25JAN mit Days &lt;= 3, also wird die Berechnung abgebrochen.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Dies ist dier erste Duration die mehrere Regeln nutzen kann. Folgende Days Regeln könnten passen: 4,6,7,8,12,14. Der Revolving vom 4/3 ist hier 3, daher gibt es keine Days=16 (4,4,4) Regel. Die grösste vorhanden Regel ist 14 (DayString=7,7) Die Tage kommen analog dem Beispiel für Duration=14. Es bleiben noch 4 Tage übrig, mit dem Startdatum=15JAN. Also müssen wir ab dem 15JAN nach einem Special suchen der passt mit Days&lt;=4, und da gibt es den 4/3. Mit EndDays kommt dann noch zusätzlich zu den Tagen 6JAN, 7JAN, 13JAN und 14JAN noch der 18JAN somit zum Abzug.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Dieser Fall funktioniert analog dem Duration=18. Die gleichen Tage kommen zum Abzug wie bei Duration=18.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Die grösste Days Regel welche hier passt ist die für 20 Tage mit dem DayString 7,7,6. Die 20 Tage werden in die Gruppen 1-7JAN, 8-14JAN und 15-20JAN aufgeteilt. Da EndDays, kommen die Tage 6JAN, 7JAN, 13JAN, 14JAN, 20JAN zum Abzug.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Die grösste passende Regel hier ist die Days=21 mit DayString 7,7,7. Daher sind die gleichen Begründungen wirksam wie im Fall Duration=20, und die Tage  6JAN, 7JAN, 13JAN, 14JAN, 20JAN, 21JAN kommen zum Abzug.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Die grösste passende Regel hier ist die Days=21, daher sind die gleichen Regeln wirksam wie für Duration=20.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Die grösste passende Regel hier ist die Days=21, daher sind die gleichen Regeln wirksam wie für Duration=20. Es gibt keine weitere Regel die ab dem 21JAN gilt für Days=2, daher kann mit der Berechnung abgebrochen werden.</t>
+  </si>
+  <si>
+    <t>MinDays, MaxDays,MinAmount,MaxAmount,Average in Verbindung mit StartDateRelevant. Dieses Beispiel zeigt die Anwendung vom EndDays. Die effektiven PerDayPrices sind vom 23JAN bis 29JAN, und mit der Regel EndDays kommen die Tage 28JAN und 29JAN zum Abzug.</t>
+  </si>
+  <si>
+    <t>MinDays, MaxDays,MinAmount,MaxAmount,Average in Verbindung mit StartDateRelevant. Dieses Beispiel zeigt die Anwendung vom StartDays. Die effektiven PerDayPrices sind vom 23JAN bis 29JAN, und mit der Regel StartDays kommen die Tage 23JAN und 24JAN zum Abzug.</t>
+  </si>
+  <si>
+    <t>MinDays, MaxDays,MinAmount,MaxAmount,Average in Verbindung mit StartDateRelevant. Dieses Beispiel zeigt die Anwendung vom MinAmount. Die effektiven PerDayPrices sind vom 23JAN bis 29JAN, die PerDayPrices Liste wird sortiert nach Preis aufsteigend und die ersten zwei Einträge aus der Liste werden für den Special genutzt.</t>
+  </si>
+  <si>
+    <t>MinDays, MaxDays,MinAmount,MaxAmount,Average in Verbindung mit StartDateRelevant. Dieses Beispiel zeigt die Anwendung vom MaxAmount. Die effektiven PerDayPrices sind vom 23JAN bis 29JAN, die PerDayPrices Liste wird sortiert nach Preis absteigend und die ersten zwei Einträge aus der Liste werden für den Special genutzt.</t>
+  </si>
+  <si>
+    <t>MinDays, MaxDays,MinAmount,MaxAmount,Average in Verbindung mit StartDateRelevant. Dieses Beispiel zeigt die Anwendung vom Average. Die effektiven PerDayPrices sind vom 23JAN bis 29JAN, es wird ein Durchschnitt der Preise gemacht, und da die Duration 7 Tage ist, und PayNights=5 wird der Average-Betrag zwei Mal abgezogen.</t>
   </si>
 </sst>
 </file>
@@ -1359,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,7 +2096,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
@@ -2095,10 +2131,10 @@
         <v>17</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -2133,10 +2169,10 @@
         <v>18</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
@@ -2171,10 +2207,10 @@
         <v>19</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -2209,10 +2245,10 @@
         <v>20</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>37</v>
       </c>
@@ -2247,10 +2283,10 @@
         <v>21</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>37</v>
       </c>
@@ -2285,10 +2321,10 @@
         <v>22</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>37</v>
       </c>
@@ -2323,10 +2359,10 @@
         <v>23</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
@@ -2361,10 +2397,10 @@
         <v>7</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>37</v>
       </c>
@@ -2399,10 +2435,10 @@
         <v>7</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
@@ -2437,10 +2473,10 @@
         <v>7</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>37</v>
       </c>
@@ -2475,10 +2511,10 @@
         <v>7</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>37</v>
       </c>
@@ -2513,7 +2549,7 @@
         <v>7</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>56</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3932,8 +3968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
mod Examples and table
</commit_message>
<xml_diff>
--- a/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
+++ b/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\github\OltSchema\BaseData\HotelExport\SpecialOffers\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
   </bookViews>
@@ -22,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="288">
   <si>
     <t>ItemType</t>
   </si>
@@ -783,18 +778,7 @@
     <t xml:space="preserve">(10.05.16-13.05.16) 10.05.16 / 510 </t>
   </si>
   <si>
-    <t xml:space="preserve">(10.05.16-13.05.16) 10.05.16 / 510 
-(14.05.16-17.05.16) 14.05.16 / 514 </t>
-  </si>
-  <si>
     <t>TUIXYA104370521</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(18.05.16-21.05.16) 18.05.16 / 518 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(11.05.16-14.05.16) 11.05.16 / 511 
-(15.05.16-18.05.16) 15.05.16 / 515 </t>
   </si>
   <si>
     <t xml:space="preserve">(12.05.16-15.05.16) 12.05.16 / 512 
@@ -817,18 +801,12 @@
 (20.05.16-23.05.16) 20.05.16 / 520 </t>
   </si>
   <si>
-    <t xml:space="preserve">(24.05.16-28.05.16) 24.05.16 / 524 </t>
-  </si>
-  <si>
     <t>TUIXYA104370525</t>
   </si>
   <si>
     <t>stay 7 pay 6</t>
   </si>
   <si>
-    <t xml:space="preserve">(17.05.16-23.05.16) 17.05.16 / 517 </t>
-  </si>
-  <si>
     <t>stay 7 pay 6 Mai Saison übergreifend</t>
   </si>
   <si>
@@ -838,39 +816,18 @@
     <t>stay 6 pay 5</t>
   </si>
   <si>
-    <t xml:space="preserve">(24.05.16-29.05.16) 24.05.16 / 524 </t>
-  </si>
-  <si>
     <t>stay 6 pay 5 Mai Saison übergreifend</t>
   </si>
   <si>
     <t>TUIXYA104370527</t>
   </si>
   <si>
-    <t xml:space="preserve">(18.05.16-24.05.16) 18.05.16 / 518 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(25.05.16-30.05.16) 25.05.16 / 525 </t>
-  </si>
-  <si>
     <t xml:space="preserve">(19.05.16-25.05.16) 19.05.16 / 519 </t>
   </si>
   <si>
     <t xml:space="preserve">(26.05.16-31.05.16) 26.05.16 / 526 </t>
   </si>
   <si>
-    <t xml:space="preserve">(20.05.16-23.05.16) 20.05.16 / 520 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(24.05.16-30.05.16) 24.05.16 / 524 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(21.05.16-24.05.16) 21.05.16 / 521 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(25.05.16-31.05.16) 25.05.16 / 525 </t>
-  </si>
-  <si>
     <t xml:space="preserve">(22.05.16-25.05.16) 22.05.16 / 522 </t>
   </si>
   <si>
@@ -884,14 +841,6 @@
   </si>
   <si>
     <t>6,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(24.05.16-29.05.16) 24.05.16 / 524 
-(30.05.16-04.06.16) 30.05.16 / 530 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(25.05.16-30.05.16) 25.05.16 / 525 
-(31.05.16-05.06.16) 31.05.16 / 531 </t>
   </si>
   <si>
     <t xml:space="preserve">(26.05.16-31.05.16) 26.05.16 / 526 
@@ -905,14 +854,6 @@
     <t>5,5</t>
   </si>
   <si>
-    <t xml:space="preserve">(28.05.16-01.06.16) 28.05.16 / 528 
-(02.06.16-06.06.16) 02.06.16 / 602 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(29.05.16-02.06.16) 29.05.16 / 529 
-(03.06.16-07.06.16) 03.06.16 / 603 </t>
-  </si>
-  <si>
     <t>Muss fragen ob Klaus die benötigt. Es gibt schon eine Beispiel</t>
   </si>
   <si>
@@ -926,6 +867,63 @@
   </si>
   <si>
     <t>Komplexere Saisonüberschneidung mit normalen Specials</t>
+  </si>
+  <si>
+    <t>AddAmount</t>
+  </si>
+  <si>
+    <t>SpecialSeq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(17.05.16-20.05.16) 17.05.16 / 517 
+(21.05.16-24.05.16) 21.05.16 / 521 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(18.05.16-21.05.16) 18.05.16 / 518 
+(22.05.16-25.05.16) 22.05.16 / 522 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(26.05.16-30.05.16) 26.05.16 / 526 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20.05.16-26.05.16) 20.05.16 / 520 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(27.05.16-01.06.16) 27.05.16 / 527 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21.05.16-27.05.16) 21.05.16 / 521 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(28.05.16-02.06.16) 28.05.16 / 528 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(24.05.16-27.05.16) 24.05.16 / 524 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(28.05.16-03.06.16) 28.05.16 / 528 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(25.05.16-28.05.16) 25.05.16 / 525 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(29.05.16-04.06.16) 29.05.16 / 529 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(28.05.16-02.06.16) 28.05.16 / 528 
+(03.06.16-08.06.16) 03.06.16 / 603 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(29.05.16-03.06.16) 29.05.16 / 529 
+(04.06.16-09.06.16) 04.06.16 / 604 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(30.05.16-03.06.16) 30.05.16 / 530 
+(04.06.16-08.06.16) 04.06.16 / 604 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(31.05.16-04.06.16) 31.05.16 / 531 
+(05.06.16-09.06.16) 05.06.16 / 605 </t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1509,131 @@
     <cellStyle name="Warnender Text" xfId="1" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="2" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="41">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1522,6 +1644,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:AN1015" totalsRowShown="0" dataDxfId="0">
+  <tableColumns count="40">
+    <tableColumn id="1" name="ItemType" dataDxfId="40"/>
+    <tableColumn id="2" name="Dest" dataDxfId="39"/>
+    <tableColumn id="3" name="ParentCode" dataDxfId="38"/>
+    <tableColumn id="4" name="ItemCode" dataDxfId="37"/>
+    <tableColumn id="5" name="MealCode" dataDxfId="36"/>
+    <tableColumn id="6" name="CurrentDate" dataDxfId="35"/>
+    <tableColumn id="7" name="Adult" dataDxfId="34"/>
+    <tableColumn id="8" name="Chd" dataDxfId="33"/>
+    <tableColumn id="9" name="Inf" dataDxfId="32"/>
+    <tableColumn id="10" name="ItemStartDate" dataDxfId="31"/>
+    <tableColumn id="11" name="Duration" dataDxfId="30"/>
+    <tableColumn id="12" name="Notes" dataDxfId="29"/>
+    <tableColumn id="13" name="DateFrom" dataDxfId="28"/>
+    <tableColumn id="14" name="DateTo" dataDxfId="27"/>
+    <tableColumn id="15" name="Days" dataDxfId="26"/>
+    <tableColumn id="16" name="DayString" dataDxfId="25"/>
+    <tableColumn id="17" name="RuleDesc" dataDxfId="24"/>
+    <tableColumn id="18" name="PayNights" dataDxfId="23"/>
+    <tableColumn id="19" name="Type" dataDxfId="22"/>
+    <tableColumn id="20" name="EffectiveSpecialDays" dataDxfId="21"/>
+    <tableColumn id="21" name="LastSpOffEndDate" dataDxfId="20"/>
+    <tableColumn id="22" name="RevolvingGroup" dataDxfId="19"/>
+    <tableColumn id="23" name="StartDateRelevant" dataDxfId="18"/>
+    <tableColumn id="24" name="EndDateRelevant" dataDxfId="17"/>
+    <tableColumn id="25" name="DescId" dataDxfId="16"/>
+    <tableColumn id="26" name="DaysBeforeDepartureFrom" dataDxfId="15"/>
+    <tableColumn id="27" name="DaysBeforeDepartureTo" dataDxfId="14"/>
+    <tableColumn id="28" name="DateBeforeDepartureFrom" dataDxfId="13"/>
+    <tableColumn id="29" name="DateBeforeDepartureTo" dataDxfId="12"/>
+    <tableColumn id="30" name="ChildAdultNr" dataDxfId="11"/>
+    <tableColumn id="31" name="ChildChildNr" dataDxfId="10"/>
+    <tableColumn id="32" name="FromDayBase" dataDxfId="9"/>
+    <tableColumn id="33" name="ToDayBase" dataDxfId="8"/>
+    <tableColumn id="34" name="Child" dataDxfId="7"/>
+    <tableColumn id="35" name="Baby" dataDxfId="6"/>
+    <tableColumn id="36" name="RuleType" dataDxfId="5"/>
+    <tableColumn id="37" name="AddAmount" dataDxfId="4"/>
+    <tableColumn id="38" name="ItemSeq" dataDxfId="3"/>
+    <tableColumn id="39" name="ParentSeq" dataDxfId="2"/>
+    <tableColumn id="40" name="SpecialSeq" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1779,7 +1949,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1789,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W89" sqref="W89"/>
+    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J81" sqref="J81:J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4505,7 +4675,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="K81" s="2">
         <v>13</v>
@@ -4540,7 +4710,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="7">
-        <v>42501</v>
+        <v>42503</v>
       </c>
       <c r="K82" s="2">
         <v>13</v>
@@ -4575,7 +4745,7 @@
         <v>0</v>
       </c>
       <c r="J83" s="7">
-        <v>42502</v>
+        <v>42504</v>
       </c>
       <c r="K83" s="2">
         <v>13</v>
@@ -4610,7 +4780,7 @@
         <v>0</v>
       </c>
       <c r="J84" s="7">
-        <v>42503</v>
+        <v>42505</v>
       </c>
       <c r="K84" s="2">
         <v>13</v>
@@ -4645,7 +4815,7 @@
         <v>0</v>
       </c>
       <c r="J85" s="7">
-        <v>42504</v>
+        <v>42506</v>
       </c>
       <c r="K85" s="2">
         <v>13</v>
@@ -4680,7 +4850,7 @@
         <v>0</v>
       </c>
       <c r="J86" s="7">
-        <v>42505</v>
+        <v>42507</v>
       </c>
       <c r="K86" s="2">
         <v>13</v>
@@ -4715,7 +4885,7 @@
         <v>0</v>
       </c>
       <c r="J87" s="7">
-        <v>42506</v>
+        <v>42508</v>
       </c>
       <c r="K87" s="2">
         <v>13</v>
@@ -4750,7 +4920,7 @@
         <v>0</v>
       </c>
       <c r="J88" s="7">
-        <v>42507</v>
+        <v>42509</v>
       </c>
       <c r="K88" s="2">
         <v>13</v>
@@ -4785,7 +4955,7 @@
         <v>0</v>
       </c>
       <c r="J89" s="7">
-        <v>42508</v>
+        <v>42510</v>
       </c>
       <c r="K89" s="2">
         <v>13</v>
@@ -4820,7 +4990,7 @@
         <v>0</v>
       </c>
       <c r="J90" s="7">
-        <v>42509</v>
+        <v>42511</v>
       </c>
       <c r="K90" s="2">
         <v>13</v>
@@ -4855,7 +5025,7 @@
         <v>0</v>
       </c>
       <c r="J91" s="7">
-        <v>42510</v>
+        <v>42512</v>
       </c>
       <c r="K91" s="2">
         <v>13</v>
@@ -4890,7 +5060,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="7">
-        <v>42511</v>
+        <v>42513</v>
       </c>
       <c r="K92" s="2">
         <v>13</v>
@@ -4925,7 +5095,7 @@
         <v>0</v>
       </c>
       <c r="J93" s="7">
-        <v>42512</v>
+        <v>42514</v>
       </c>
       <c r="K93" s="2">
         <v>13</v>
@@ -4960,7 +5130,7 @@
         <v>0</v>
       </c>
       <c r="J94" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="K94" s="2">
         <v>13</v>
@@ -4995,7 +5165,7 @@
         <v>0</v>
       </c>
       <c r="J95" s="7">
-        <v>42514</v>
+        <v>42516</v>
       </c>
       <c r="K95" s="2">
         <v>13</v>
@@ -5030,7 +5200,7 @@
         <v>0</v>
       </c>
       <c r="J96" s="7">
-        <v>42515</v>
+        <v>42517</v>
       </c>
       <c r="K96" s="2">
         <v>13</v>
@@ -5065,7 +5235,7 @@
         <v>0</v>
       </c>
       <c r="J97" s="7">
-        <v>42516</v>
+        <v>42518</v>
       </c>
       <c r="K97" s="2">
         <v>13</v>
@@ -5100,7 +5270,7 @@
         <v>0</v>
       </c>
       <c r="J98" s="7">
-        <v>42517</v>
+        <v>42519</v>
       </c>
       <c r="K98" s="2">
         <v>13</v>
@@ -5135,7 +5305,7 @@
         <v>0</v>
       </c>
       <c r="J99" s="7">
-        <v>42518</v>
+        <v>42520</v>
       </c>
       <c r="K99" s="2">
         <v>13</v>
@@ -5170,7 +5340,7 @@
         <v>0</v>
       </c>
       <c r="J100" s="7">
-        <v>42519</v>
+        <v>42521</v>
       </c>
       <c r="K100" s="2">
         <v>13</v>
@@ -5184,50 +5354,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN111"/>
+  <dimension ref="A1:AN110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L71" sqref="L71"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P108" sqref="P108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="2"/>
-    <col min="2" max="2" width="5" style="2"/>
-    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="2"/>
-    <col min="6" max="6" width="11.85546875" style="2"/>
-    <col min="7" max="7" width="5.85546875" style="2"/>
-    <col min="8" max="8" width="4.42578125" style="2"/>
-    <col min="9" max="9" width="3.42578125" style="2"/>
-    <col min="10" max="10" width="13.42578125" style="2"/>
-    <col min="11" max="11" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="11.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8" style="2" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="47" style="6" customWidth="1"/>
-    <col min="13" max="14" width="10.140625" style="2"/>
-    <col min="15" max="15" width="5.140625" style="2"/>
-    <col min="16" max="16" width="9.42578125" style="2"/>
+    <col min="13" max="13" width="11.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="2"/>
+    <col min="15" max="15" width="7.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="2" customWidth="1"/>
     <col min="17" max="17" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" style="2"/>
+    <col min="18" max="18" width="12" style="2" customWidth="1"/>
     <col min="19" max="19" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="39.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17" style="2"/>
-    <col min="22" max="22" width="15.140625" style="2"/>
-    <col min="23" max="23" width="17.28515625" style="2"/>
-    <col min="24" max="24" width="16.42578125" style="2"/>
+    <col min="21" max="21" width="19" style="2" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" style="2" customWidth="1"/>
     <col min="25" max="25" width="47.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25" style="2"/>
-    <col min="27" max="27" width="22.5703125" style="2"/>
-    <col min="28" max="28" width="25" style="2"/>
-    <col min="29" max="29" width="22.5703125" style="2"/>
-    <col min="30" max="30" width="12.5703125" style="2"/>
-    <col min="31" max="31" width="12.28515625" style="2"/>
-    <col min="32" max="32" width="13" style="2"/>
-    <col min="33" max="33" width="10.5703125" style="2"/>
-    <col min="34" max="34" width="5.5703125" style="2"/>
-    <col min="35" max="35" width="5.28515625" style="2"/>
-    <col min="36" max="36" width="9.28515625" style="2"/>
-    <col min="37" max="37" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.85546875" style="2" customWidth="1"/>
+    <col min="27" max="27" width="24.42578125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="26.85546875" style="2" customWidth="1"/>
+    <col min="29" max="29" width="24.42578125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="14.7109375" style="2" customWidth="1"/>
+    <col min="31" max="31" width="14.42578125" style="2" customWidth="1"/>
+    <col min="32" max="32" width="15.140625" style="2" customWidth="1"/>
+    <col min="33" max="33" width="12.7109375" style="2" customWidth="1"/>
+    <col min="34" max="34" width="7.7109375" style="2" customWidth="1"/>
+    <col min="35" max="35" width="7.42578125" style="2" customWidth="1"/>
+    <col min="36" max="36" width="11.42578125" style="2" customWidth="1"/>
+    <col min="37" max="37" width="13.85546875" style="2" customWidth="1"/>
     <col min="38" max="38" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -5344,11 +5515,17 @@
       <c r="AJ1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AK1" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="AL1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AM1" s="11" t="s">
         <v>35</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:40" ht="60" x14ac:dyDescent="0.25">
@@ -13145,16 +13322,16 @@
         <v>0</v>
       </c>
       <c r="J83" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="K83" s="2">
         <v>13</v>
       </c>
       <c r="M83" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N83" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O83" s="2">
         <v>8</v>
@@ -13172,10 +13349,10 @@
         <v>97</v>
       </c>
       <c r="T83" s="6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="U83" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="V83" s="2">
         <v>2</v>
@@ -13220,27 +13397,54 @@
         <v>44</v>
       </c>
       <c r="AN83" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="84" spans="1:40" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="84" spans="1:40" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B84" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D84" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="E84" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G84" s="2">
+        <v>1</v>
+      </c>
+      <c r="H84" s="2">
+        <v>0</v>
+      </c>
+      <c r="I84" s="2">
+        <v>0</v>
+      </c>
+      <c r="J84" s="7">
+        <v>42503</v>
+      </c>
+      <c r="K84" s="2">
+        <v>13</v>
+      </c>
       <c r="M84" s="7">
-        <v>42496</v>
+        <v>42502</v>
       </c>
       <c r="N84" s="7">
-        <v>42500</v>
+        <v>42515</v>
       </c>
       <c r="O84" s="2">
-        <v>4</v>
-      </c>
-      <c r="P84" s="2">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="P84" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="Q84" s="2" t="s">
         <v>51</v>
@@ -13255,10 +13459,10 @@
         <v>245</v>
       </c>
       <c r="U84" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="V84" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W84" s="2" t="s">
         <v>42</v>
@@ -13300,7 +13504,7 @@
         <v>44</v>
       </c>
       <c r="AN84" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -13332,16 +13536,16 @@
         <v>0</v>
       </c>
       <c r="J85" s="7">
-        <v>42501</v>
+        <v>42504</v>
       </c>
       <c r="K85" s="2">
         <v>13</v>
       </c>
       <c r="M85" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N85" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O85" s="2">
         <v>8</v>
@@ -13362,7 +13566,7 @@
         <v>246</v>
       </c>
       <c r="U85" s="7">
-        <v>42513</v>
+        <v>42530</v>
       </c>
       <c r="V85" s="2">
         <v>2</v>
@@ -13407,7 +13611,7 @@
         <v>44</v>
       </c>
       <c r="AN85" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -13439,16 +13643,16 @@
         <v>0</v>
       </c>
       <c r="J86" s="7">
-        <v>42502</v>
+        <v>42505</v>
       </c>
       <c r="K86" s="2">
         <v>13</v>
       </c>
       <c r="M86" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N86" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O86" s="2">
         <v>8</v>
@@ -13469,7 +13673,7 @@
         <v>247</v>
       </c>
       <c r="U86" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V86" s="2">
         <v>2</v>
@@ -13514,7 +13718,7 @@
         <v>44</v>
       </c>
       <c r="AN86" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="87" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -13546,16 +13750,16 @@
         <v>0</v>
       </c>
       <c r="J87" s="7">
-        <v>42503</v>
+        <v>42506</v>
       </c>
       <c r="K87" s="2">
         <v>13</v>
       </c>
       <c r="M87" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N87" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O87" s="2">
         <v>8</v>
@@ -13576,7 +13780,7 @@
         <v>248</v>
       </c>
       <c r="U87" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V87" s="2">
         <v>2</v>
@@ -13621,7 +13825,7 @@
         <v>44</v>
       </c>
       <c r="AN87" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="88" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -13653,16 +13857,16 @@
         <v>0</v>
       </c>
       <c r="J88" s="7">
-        <v>42504</v>
+        <v>42507</v>
       </c>
       <c r="K88" s="2">
         <v>13</v>
       </c>
       <c r="M88" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N88" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O88" s="2">
         <v>8</v>
@@ -13680,10 +13884,10 @@
         <v>97</v>
       </c>
       <c r="T88" s="6" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="U88" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V88" s="2">
         <v>2</v>
@@ -13728,7 +13932,7 @@
         <v>44</v>
       </c>
       <c r="AN88" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="89" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -13760,16 +13964,16 @@
         <v>0</v>
       </c>
       <c r="J89" s="7">
-        <v>42505</v>
+        <v>42508</v>
       </c>
       <c r="K89" s="2">
         <v>13</v>
       </c>
       <c r="M89" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N89" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O89" s="2">
         <v>8</v>
@@ -13787,10 +13991,10 @@
         <v>97</v>
       </c>
       <c r="T89" s="6" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="U89" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V89" s="2">
         <v>2</v>
@@ -13835,69 +14039,39 @@
         <v>44</v>
       </c>
       <c r="AN89" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="90" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="90" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G90" s="2">
-        <v>1</v>
-      </c>
-      <c r="H90" s="2">
-        <v>0</v>
-      </c>
-      <c r="I90" s="2">
-        <v>0</v>
-      </c>
-      <c r="J90" s="7">
-        <v>42506</v>
-      </c>
-      <c r="K90" s="2">
-        <v>13</v>
-      </c>
       <c r="M90" s="7">
-        <v>42500</v>
+        <v>42516</v>
       </c>
       <c r="N90" s="7">
-        <v>42513</v>
+        <v>42530</v>
       </c>
       <c r="O90" s="2">
-        <v>8</v>
-      </c>
-      <c r="P90" s="2" t="s">
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="P90" s="2">
+        <v>5</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
       <c r="R90" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S90" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T90" s="6" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="U90" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V90" s="2">
         <v>2</v>
@@ -13909,7 +14083,7 @@
         <v>42</v>
       </c>
       <c r="Y90" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AD90" s="2">
         <v>0</v>
@@ -13918,10 +14092,10 @@
         <v>0</v>
       </c>
       <c r="AF90" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG90" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH90" s="2">
         <v>0</v>
@@ -13942,42 +14116,69 @@
         <v>44</v>
       </c>
       <c r="AN90" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B91" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D91" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="E91" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G91" s="2">
+        <v>1</v>
+      </c>
+      <c r="H91" s="2">
+        <v>0</v>
+      </c>
+      <c r="I91" s="2">
+        <v>0</v>
+      </c>
+      <c r="J91" s="7">
+        <v>42509</v>
+      </c>
+      <c r="K91" s="2">
+        <v>13</v>
+      </c>
       <c r="M91" s="7">
-        <v>42514</v>
+        <v>42502</v>
       </c>
       <c r="N91" s="7">
-        <v>42528</v>
+        <v>42515</v>
       </c>
       <c r="O91" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P91" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>169</v>
+        <v>250</v>
       </c>
       <c r="R91" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S91" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T91" s="6" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="U91" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V91" s="2">
         <v>2</v>
@@ -13989,7 +14190,7 @@
         <v>42</v>
       </c>
       <c r="Y91" s="2" t="s">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="AD91" s="2">
         <v>0</v>
@@ -13998,10 +14199,10 @@
         <v>0</v>
       </c>
       <c r="AF91" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AG91" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AH91" s="2">
         <v>0</v>
@@ -14022,69 +14223,39 @@
         <v>44</v>
       </c>
       <c r="AN91" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="92" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G92" s="2">
-        <v>1</v>
-      </c>
-      <c r="H92" s="2">
-        <v>0</v>
-      </c>
-      <c r="I92" s="2">
-        <v>0</v>
-      </c>
-      <c r="J92" s="7">
-        <v>42507</v>
-      </c>
-      <c r="K92" s="2">
-        <v>13</v>
-      </c>
       <c r="M92" s="7">
-        <v>42500</v>
+        <v>42516</v>
       </c>
       <c r="N92" s="7">
-        <v>42513</v>
+        <v>42530</v>
       </c>
       <c r="O92" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P92" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q92" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R92" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S92" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T92" s="6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="U92" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V92" s="2">
         <v>2</v>
@@ -14096,7 +14267,7 @@
         <v>42</v>
       </c>
       <c r="Y92" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AD92" s="2">
         <v>0</v>
@@ -14105,10 +14276,10 @@
         <v>0</v>
       </c>
       <c r="AF92" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG92" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH92" s="2">
         <v>0</v>
@@ -14129,42 +14300,69 @@
         <v>44</v>
       </c>
       <c r="AN92" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="93" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B93" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D93" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="E93" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G93" s="2">
+        <v>1</v>
+      </c>
+      <c r="H93" s="2">
+        <v>0</v>
+      </c>
+      <c r="I93" s="2">
+        <v>0</v>
+      </c>
+      <c r="J93" s="7">
+        <v>42510</v>
+      </c>
+      <c r="K93" s="2">
+        <v>13</v>
+      </c>
       <c r="M93" s="7">
-        <v>42514</v>
+        <v>42502</v>
       </c>
       <c r="N93" s="7">
-        <v>42528</v>
+        <v>42515</v>
       </c>
       <c r="O93" s="2">
+        <v>7</v>
+      </c>
+      <c r="P93" s="2">
+        <v>7</v>
+      </c>
+      <c r="Q93" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="R93" s="2">
         <v>6</v>
-      </c>
-      <c r="P93" s="2">
-        <v>6</v>
-      </c>
-      <c r="Q93" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="R93" s="2">
-        <v>5</v>
       </c>
       <c r="S93" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T93" s="6" t="s">
-        <v>259</v>
+        <v>276</v>
       </c>
       <c r="U93" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V93" s="2">
         <v>2</v>
@@ -14176,7 +14374,7 @@
         <v>42</v>
       </c>
       <c r="Y93" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="AD93" s="2">
         <v>0</v>
@@ -14185,10 +14383,10 @@
         <v>0</v>
       </c>
       <c r="AF93" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AG93" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH93" s="2">
         <v>0</v>
@@ -14209,69 +14407,39 @@
         <v>44</v>
       </c>
       <c r="AN93" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G94" s="2">
-        <v>1</v>
-      </c>
-      <c r="H94" s="2">
-        <v>0</v>
-      </c>
-      <c r="I94" s="2">
-        <v>0</v>
-      </c>
-      <c r="J94" s="7">
-        <v>42508</v>
-      </c>
-      <c r="K94" s="2">
-        <v>13</v>
-      </c>
       <c r="M94" s="7">
-        <v>42500</v>
+        <v>42516</v>
       </c>
       <c r="N94" s="7">
-        <v>42513</v>
+        <v>42530</v>
       </c>
       <c r="O94" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P94" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q94" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R94" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S94" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T94" s="6" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="U94" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V94" s="2">
         <v>2</v>
@@ -14283,7 +14451,7 @@
         <v>42</v>
       </c>
       <c r="Y94" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AD94" s="2">
         <v>0</v>
@@ -14292,10 +14460,10 @@
         <v>0</v>
       </c>
       <c r="AF94" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG94" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH94" s="2">
         <v>0</v>
@@ -14316,42 +14484,69 @@
         <v>44</v>
       </c>
       <c r="AN94" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="95" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B95" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D95" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="E95" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G95" s="2">
+        <v>1</v>
+      </c>
+      <c r="H95" s="2">
+        <v>0</v>
+      </c>
+      <c r="I95" s="2">
+        <v>0</v>
+      </c>
+      <c r="J95" s="7">
+        <v>42511</v>
+      </c>
+      <c r="K95" s="2">
+        <v>13</v>
+      </c>
       <c r="M95" s="7">
-        <v>42514</v>
+        <v>42502</v>
       </c>
       <c r="N95" s="7">
-        <v>42528</v>
+        <v>42515</v>
       </c>
       <c r="O95" s="2">
+        <v>7</v>
+      </c>
+      <c r="P95" s="2">
+        <v>7</v>
+      </c>
+      <c r="Q95" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="R95" s="2">
         <v>6</v>
-      </c>
-      <c r="P95" s="2">
-        <v>6</v>
-      </c>
-      <c r="Q95" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="R95" s="2">
-        <v>5</v>
       </c>
       <c r="S95" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T95" s="6" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="U95" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V95" s="2">
         <v>2</v>
@@ -14363,7 +14558,7 @@
         <v>42</v>
       </c>
       <c r="Y95" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="AD95" s="2">
         <v>0</v>
@@ -14372,10 +14567,10 @@
         <v>0</v>
       </c>
       <c r="AF95" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AG95" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH95" s="2">
         <v>0</v>
@@ -14396,69 +14591,39 @@
         <v>44</v>
       </c>
       <c r="AN95" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="96" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G96" s="2">
-        <v>1</v>
-      </c>
-      <c r="H96" s="2">
-        <v>0</v>
-      </c>
-      <c r="I96" s="2">
-        <v>0</v>
-      </c>
-      <c r="J96" s="7">
-        <v>42509</v>
-      </c>
-      <c r="K96" s="2">
-        <v>13</v>
-      </c>
       <c r="M96" s="7">
-        <v>42500</v>
+        <v>42516</v>
       </c>
       <c r="N96" s="7">
-        <v>42513</v>
+        <v>42530</v>
       </c>
       <c r="O96" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P96" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q96" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R96" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S96" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T96" s="6" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="U96" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V96" s="2">
         <v>2</v>
@@ -14470,7 +14635,7 @@
         <v>42</v>
       </c>
       <c r="Y96" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AD96" s="2">
         <v>0</v>
@@ -14479,10 +14644,10 @@
         <v>0</v>
       </c>
       <c r="AF96" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG96" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH96" s="2">
         <v>0</v>
@@ -14503,42 +14668,69 @@
         <v>44</v>
       </c>
       <c r="AN96" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="97" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B97" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D97" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="E97" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G97" s="2">
+        <v>1</v>
+      </c>
+      <c r="H97" s="2">
+        <v>0</v>
+      </c>
+      <c r="I97" s="2">
+        <v>0</v>
+      </c>
+      <c r="J97" s="7">
+        <v>42512</v>
+      </c>
+      <c r="K97" s="2">
+        <v>13</v>
+      </c>
       <c r="M97" s="7">
-        <v>42514</v>
+        <v>42502</v>
       </c>
       <c r="N97" s="7">
-        <v>42528</v>
+        <v>42515</v>
       </c>
       <c r="O97" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P97" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q97" s="2" t="s">
-        <v>258</v>
+        <v>51</v>
       </c>
       <c r="R97" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S97" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T97" s="6" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="U97" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V97" s="2">
         <v>2</v>
@@ -14550,7 +14742,7 @@
         <v>42</v>
       </c>
       <c r="Y97" s="2" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
       <c r="AD97" s="2">
         <v>0</v>
@@ -14559,10 +14751,10 @@
         <v>0</v>
       </c>
       <c r="AF97" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AG97" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AH97" s="2">
         <v>0</v>
@@ -14583,69 +14775,39 @@
         <v>44</v>
       </c>
       <c r="AN97" s="2" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G98" s="2">
-        <v>1</v>
-      </c>
-      <c r="H98" s="2">
-        <v>0</v>
-      </c>
-      <c r="I98" s="2">
-        <v>0</v>
-      </c>
-      <c r="J98" s="7">
-        <v>42510</v>
-      </c>
-      <c r="K98" s="2">
-        <v>13</v>
-      </c>
       <c r="M98" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N98" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O98" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P98" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q98" s="2" t="s">
-        <v>51</v>
+        <v>250</v>
       </c>
       <c r="R98" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S98" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T98" s="6" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="U98" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V98" s="2">
         <v>2</v>
@@ -14657,7 +14819,7 @@
         <v>42</v>
       </c>
       <c r="Y98" s="2" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="AD98" s="2">
         <v>0</v>
@@ -14666,10 +14828,10 @@
         <v>0</v>
       </c>
       <c r="AF98" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AG98" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AH98" s="2">
         <v>0</v>
@@ -14690,42 +14852,69 @@
         <v>44</v>
       </c>
       <c r="AN98" s="2" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="99" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B99" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D99" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="E99" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G99" s="2">
+        <v>1</v>
+      </c>
+      <c r="H99" s="2">
+        <v>0</v>
+      </c>
+      <c r="I99" s="2">
+        <v>0</v>
+      </c>
+      <c r="J99" s="7">
+        <v>42513</v>
+      </c>
+      <c r="K99" s="2">
+        <v>13</v>
+      </c>
       <c r="M99" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N99" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O99" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P99" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Q99" s="2" t="s">
-        <v>254</v>
+        <v>51</v>
       </c>
       <c r="R99" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S99" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T99" s="6" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="U99" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V99" s="2">
         <v>2</v>
@@ -14737,7 +14926,7 @@
         <v>42</v>
       </c>
       <c r="Y99" s="2" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="AD99" s="2">
         <v>0</v>
@@ -14746,10 +14935,10 @@
         <v>0</v>
       </c>
       <c r="AF99" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AG99" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AH99" s="2">
         <v>0</v>
@@ -14770,69 +14959,39 @@
         <v>44</v>
       </c>
       <c r="AN99" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="100" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G100" s="2">
-        <v>1</v>
-      </c>
-      <c r="H100" s="2">
-        <v>0</v>
-      </c>
-      <c r="I100" s="2">
-        <v>0</v>
-      </c>
-      <c r="J100" s="7">
-        <v>42511</v>
-      </c>
-      <c r="K100" s="2">
-        <v>13</v>
-      </c>
       <c r="M100" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N100" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O100" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P100" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q100" s="2" t="s">
-        <v>51</v>
+        <v>250</v>
       </c>
       <c r="R100" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T100" s="6" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="U100" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V100" s="2">
         <v>2</v>
@@ -14844,7 +15003,7 @@
         <v>42</v>
       </c>
       <c r="Y100" s="2" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="AD100" s="2">
         <v>0</v>
@@ -14853,10 +15012,10 @@
         <v>0</v>
       </c>
       <c r="AF100" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AG100" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AH100" s="2">
         <v>0</v>
@@ -14877,42 +15036,69 @@
         <v>44</v>
       </c>
       <c r="AN100" s="2" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="101" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B101" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D101" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="E101" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G101" s="2">
+        <v>1</v>
+      </c>
+      <c r="H101" s="2">
+        <v>0</v>
+      </c>
+      <c r="I101" s="2">
+        <v>0</v>
+      </c>
+      <c r="J101" s="7">
+        <v>42514</v>
+      </c>
+      <c r="K101" s="2">
+        <v>13</v>
+      </c>
       <c r="M101" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N101" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O101" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P101" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Q101" s="2" t="s">
-        <v>254</v>
+        <v>51</v>
       </c>
       <c r="R101" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S101" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T101" s="6" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="U101" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V101" s="2">
         <v>2</v>
@@ -14924,7 +15110,7 @@
         <v>42</v>
       </c>
       <c r="Y101" s="2" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="AD101" s="2">
         <v>0</v>
@@ -14933,10 +15119,10 @@
         <v>0</v>
       </c>
       <c r="AF101" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AG101" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AH101" s="2">
         <v>0</v>
@@ -14957,69 +15143,39 @@
         <v>44</v>
       </c>
       <c r="AN101" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G102" s="2">
-        <v>1</v>
-      </c>
-      <c r="H102" s="2">
-        <v>0</v>
-      </c>
-      <c r="I102" s="2">
-        <v>0</v>
-      </c>
-      <c r="J102" s="7">
-        <v>42512</v>
-      </c>
-      <c r="K102" s="2">
-        <v>13</v>
-      </c>
       <c r="M102" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N102" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O102" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P102" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q102" s="2" t="s">
-        <v>51</v>
+        <v>250</v>
       </c>
       <c r="R102" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S102" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T102" s="6" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="U102" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V102" s="2">
         <v>2</v>
@@ -15031,7 +15187,7 @@
         <v>42</v>
       </c>
       <c r="Y102" s="2" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="AD102" s="2">
         <v>0</v>
@@ -15040,10 +15196,10 @@
         <v>0</v>
       </c>
       <c r="AF102" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AG102" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AH102" s="2">
         <v>0</v>
@@ -15064,42 +15220,69 @@
         <v>44</v>
       </c>
       <c r="AN102" s="2" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="103" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B103" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D103" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="E103" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G103" s="2">
+        <v>1</v>
+      </c>
+      <c r="H103" s="2">
+        <v>0</v>
+      </c>
+      <c r="I103" s="2">
+        <v>0</v>
+      </c>
+      <c r="J103" s="7">
+        <v>42515</v>
+      </c>
+      <c r="K103" s="2">
+        <v>13</v>
+      </c>
       <c r="M103" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N103" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O103" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P103" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Q103" s="2" t="s">
-        <v>254</v>
+        <v>51</v>
       </c>
       <c r="R103" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S103" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T103" s="6" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="U103" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V103" s="2">
         <v>2</v>
@@ -15111,7 +15294,7 @@
         <v>42</v>
       </c>
       <c r="Y103" s="2" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="AD103" s="2">
         <v>0</v>
@@ -15120,10 +15303,10 @@
         <v>0</v>
       </c>
       <c r="AF103" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AG103" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AH103" s="2">
         <v>0</v>
@@ -15144,69 +15327,39 @@
         <v>44</v>
       </c>
       <c r="AN103" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="104" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G104" s="2">
-        <v>1</v>
-      </c>
-      <c r="H104" s="2">
-        <v>0</v>
-      </c>
-      <c r="I104" s="2">
-        <v>0</v>
-      </c>
-      <c r="J104" s="7">
-        <v>42513</v>
-      </c>
-      <c r="K104" s="2">
-        <v>13</v>
-      </c>
       <c r="M104" s="7">
-        <v>42500</v>
+        <v>42502</v>
       </c>
       <c r="N104" s="7">
-        <v>42513</v>
+        <v>42515</v>
       </c>
       <c r="O104" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P104" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q104" s="2" t="s">
-        <v>51</v>
+        <v>250</v>
       </c>
       <c r="R104" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S104" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T104" s="6" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="U104" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V104" s="2">
         <v>2</v>
@@ -15218,7 +15371,7 @@
         <v>42</v>
       </c>
       <c r="Y104" s="2" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="AD104" s="2">
         <v>0</v>
@@ -15227,10 +15380,10 @@
         <v>0</v>
       </c>
       <c r="AF104" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AG104" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AH104" s="2">
         <v>0</v>
@@ -15251,42 +15404,69 @@
         <v>44</v>
       </c>
       <c r="AN104" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="105" spans="1:40" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="105" spans="1:40" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B105" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D105" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="E105" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G105" s="2">
+        <v>1</v>
+      </c>
+      <c r="H105" s="2">
+        <v>0</v>
+      </c>
+      <c r="I105" s="2">
+        <v>0</v>
+      </c>
+      <c r="J105" s="7">
+        <v>42516</v>
+      </c>
+      <c r="K105" s="2">
+        <v>13</v>
+      </c>
       <c r="M105" s="7">
-        <v>42500</v>
+        <v>42516</v>
       </c>
       <c r="N105" s="7">
-        <v>42513</v>
+        <v>42530</v>
       </c>
       <c r="O105" s="2">
-        <v>7</v>
-      </c>
-      <c r="P105" s="2">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="P105" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="Q105" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R105" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S105" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T105" s="6" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="U105" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V105" s="2">
         <v>2</v>
@@ -15298,7 +15478,7 @@
         <v>42</v>
       </c>
       <c r="Y105" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AD105" s="2">
         <v>0</v>
@@ -15307,10 +15487,10 @@
         <v>0</v>
       </c>
       <c r="AF105" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG105" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH105" s="2">
         <v>0</v>
@@ -15331,7 +15511,7 @@
         <v>44</v>
       </c>
       <c r="AN105" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="106" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -15363,25 +15543,25 @@
         <v>0</v>
       </c>
       <c r="J106" s="7">
-        <v>42514</v>
+        <v>42517</v>
       </c>
       <c r="K106" s="2">
         <v>13</v>
       </c>
       <c r="M106" s="7">
-        <v>42514</v>
+        <v>42516</v>
       </c>
       <c r="N106" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="O106" s="2">
         <v>12</v>
       </c>
       <c r="P106" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="Q106" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="R106" s="2">
         <v>5</v>
@@ -15390,10 +15570,10 @@
         <v>97</v>
       </c>
       <c r="T106" s="6" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="U106" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V106" s="2">
         <v>2</v>
@@ -15405,7 +15585,7 @@
         <v>42</v>
       </c>
       <c r="Y106" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AD106" s="2">
         <v>0</v>
@@ -15438,7 +15618,7 @@
         <v>44</v>
       </c>
       <c r="AN106" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="107" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -15470,25 +15650,25 @@
         <v>0</v>
       </c>
       <c r="J107" s="7">
-        <v>42515</v>
+        <v>42518</v>
       </c>
       <c r="K107" s="2">
         <v>13</v>
       </c>
       <c r="M107" s="7">
-        <v>42514</v>
+        <v>42516</v>
       </c>
       <c r="N107" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="O107" s="2">
         <v>12</v>
       </c>
       <c r="P107" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="Q107" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="R107" s="2">
         <v>5</v>
@@ -15497,10 +15677,10 @@
         <v>97</v>
       </c>
       <c r="T107" s="6" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="U107" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V107" s="2">
         <v>2</v>
@@ -15512,7 +15692,7 @@
         <v>42</v>
       </c>
       <c r="Y107" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AD107" s="2">
         <v>0</v>
@@ -15545,7 +15725,7 @@
         <v>44</v>
       </c>
       <c r="AN107" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="108" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -15577,25 +15757,25 @@
         <v>0</v>
       </c>
       <c r="J108" s="7">
-        <v>42516</v>
+        <v>42519</v>
       </c>
       <c r="K108" s="2">
         <v>13</v>
       </c>
       <c r="M108" s="7">
-        <v>42514</v>
+        <v>42516</v>
       </c>
       <c r="N108" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="O108" s="2">
         <v>12</v>
       </c>
       <c r="P108" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="Q108" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="R108" s="2">
         <v>5</v>
@@ -15604,10 +15784,10 @@
         <v>97</v>
       </c>
       <c r="T108" s="6" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="U108" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V108" s="2">
         <v>2</v>
@@ -15619,7 +15799,7 @@
         <v>42</v>
       </c>
       <c r="Y108" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AD108" s="2">
         <v>0</v>
@@ -15652,7 +15832,7 @@
         <v>44</v>
       </c>
       <c r="AN108" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="109" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -15684,37 +15864,37 @@
         <v>0</v>
       </c>
       <c r="J109" s="7">
-        <v>42517</v>
+        <v>42520</v>
       </c>
       <c r="K109" s="2">
         <v>13</v>
       </c>
       <c r="M109" s="7">
-        <v>42514</v>
+        <v>42516</v>
       </c>
       <c r="N109" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="O109" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P109" s="2" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="Q109" s="2" t="s">
-        <v>258</v>
+        <v>169</v>
       </c>
       <c r="R109" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S109" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T109" s="6" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="U109" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V109" s="2">
         <v>2</v>
@@ -15726,7 +15906,7 @@
         <v>42</v>
       </c>
       <c r="Y109" s="2" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="AD109" s="2">
         <v>0</v>
@@ -15735,10 +15915,10 @@
         <v>0</v>
       </c>
       <c r="AF109" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AG109" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AH109" s="2">
         <v>0</v>
@@ -15759,7 +15939,7 @@
         <v>44</v>
       </c>
       <c r="AN109" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:40" ht="30" x14ac:dyDescent="0.25">
@@ -15791,22 +15971,22 @@
         <v>0</v>
       </c>
       <c r="J110" s="7">
-        <v>42518</v>
+        <v>42521</v>
       </c>
       <c r="K110" s="2">
         <v>13</v>
       </c>
       <c r="M110" s="7">
-        <v>42514</v>
+        <v>42516</v>
       </c>
       <c r="N110" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="O110" s="2">
         <v>10</v>
       </c>
       <c r="P110" s="2" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="Q110" s="2" t="s">
         <v>169</v>
@@ -15818,10 +15998,10 @@
         <v>97</v>
       </c>
       <c r="T110" s="6" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="U110" s="7">
-        <v>42528</v>
+        <v>42530</v>
       </c>
       <c r="V110" s="2">
         <v>2</v>
@@ -15866,119 +16046,15 @@
         <v>44</v>
       </c>
       <c r="AN110" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="111" spans="1:40" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G111" s="2">
-        <v>1</v>
-      </c>
-      <c r="H111" s="2">
-        <v>0</v>
-      </c>
-      <c r="I111" s="2">
-        <v>0</v>
-      </c>
-      <c r="J111" s="7">
-        <v>42519</v>
-      </c>
-      <c r="K111" s="2">
-        <v>13</v>
-      </c>
-      <c r="M111" s="7">
-        <v>42514</v>
-      </c>
-      <c r="N111" s="7">
-        <v>42528</v>
-      </c>
-      <c r="O111" s="2">
-        <v>10</v>
-      </c>
-      <c r="P111" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q111" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="R111" s="2">
-        <v>4</v>
-      </c>
-      <c r="S111" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="T111" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="U111" s="7">
-        <v>42528</v>
-      </c>
-      <c r="V111" s="2">
-        <v>2</v>
-      </c>
-      <c r="W111" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X111" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y111" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="AD111" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE111" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF111" s="2">
-        <v>5</v>
-      </c>
-      <c r="AG111" s="2">
-        <v>5</v>
-      </c>
-      <c r="AH111" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI111" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ111" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK111" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL111" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM111" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN111" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -19027,7 +19103,7 @@
         <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -19037,12 +19113,12 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -19052,12 +19128,12 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -19070,7 +19146,7 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -19088,7 +19164,7 @@
         <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -19136,7 +19212,7 @@
         <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -19144,7 +19220,7 @@
         <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -19152,7 +19228,7 @@
         <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -19160,7 +19236,7 @@
         <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -19168,7 +19244,7 @@
         <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SpecialOffer examples and docs
</commit_message>
<xml_diff>
--- a/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
+++ b/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="261">
   <si>
     <t>ItemType</t>
   </si>
@@ -841,6 +841,15 @@
   </si>
   <si>
     <t>Komplexere Saisonüberschneidungen. Dies ist dann wieder ein einfacher Fall. Das ItemStartDate 26MAY ItemEndDate 7JUN. Folgende Days Regeln gibt es in der neuen Saison: 5,6,10,12. Days = 12 &lt;= Duration = 13, und ist die grösste passende Regel, kann also angewendet werden. Da Type = StartDays und DayString = 6,6 gibt es zwei Gruppen: 26MAY-31MAY und 1JUN-6JUN. Die Special-Tage sind also 26MAY und 1JUN.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Hier gibt es nur den 4/3 mit Days=4 welcher zum Tragen kommt. Da Type=EndDays ist der 4JAN der Special-Tag.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving und unterschiedlicher Duration. Hier kommt nur der 4/3 zum Tragen. Analog wie dem 4 Tage Beispiel kommt der 4JAN zum Tragen. Obwohl ich mehr Tage Stay habe als der Special passt einfach kein Special besser in die 5 Tage als der 4/3.</t>
+  </si>
+  <si>
+    <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving=3 und unterschiedlicher Duration. Da es keine SpecialOffer gibt mit Days&lt;=3, kommt hier kein Special zum Tragen. Die Beispiele 01.01.2016 mit Duration 3 bis 23 sollen helfen zu verstehen wie DayString in Verbindung mit Days funktioniert, und wie ein Revolving funktioniert.</t>
   </si>
 </sst>
 </file>
@@ -17891,8 +17900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18061,7 +18070,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>36</v>
       </c>
@@ -18096,7 +18105,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>99</v>
+        <v>260</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
@@ -18166,7 +18175,7 @@
         <v>4</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>100</v>
+        <v>258</v>
       </c>
       <c r="M3" s="13">
         <v>42370</v>
@@ -18249,7 +18258,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -18284,7 +18293,7 @@
         <v>5</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>101</v>
+        <v>259</v>
       </c>
       <c r="M4" s="13">
         <v>42370</v>

</xml_diff>

<commit_message>
Finalized the SpecialOffer examples
</commit_message>
<xml_diff>
--- a/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
+++ b/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="279">
   <si>
     <t>ItemType</t>
   </si>
@@ -851,6 +851,60 @@
   <si>
     <t>Gemischte 7,6/5 and 4/3 in der gleichen Saison mit Revolving=3 und unterschiedlicher Duration. Da es keine SpecialOffer gibt mit Days&lt;=3, kommt hier kein Special zum Tragen. Die Beispiele 01.01.2016 mit Duration 3 bis 23 sollen helfen zu verstehen wie DayString in Verbindung mit Days funktioniert, und wie ein Revolving funktioniert.</t>
   </si>
+  <si>
+    <t>SZM</t>
+  </si>
+  <si>
+    <t>NAMLOD</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>stay 3 pay 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(01.01.16-03.01.16) 03.01.16 / 66 </t>
+  </si>
+  <si>
+    <t>SO ADT 3/2</t>
+  </si>
+  <si>
+    <t>TUIXYZ50502</t>
+  </si>
+  <si>
+    <t>TUIXYZ20928</t>
+  </si>
+  <si>
+    <t>TUIXYA44542716</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(01.01.16-03.01.16) 03.01.16 / 25 </t>
+  </si>
+  <si>
+    <t>SO CHD 3/2 Kind 1</t>
+  </si>
+  <si>
+    <t>TUIXYZ528517</t>
+  </si>
+  <si>
+    <t>SO CHD 3/2 Kind 2</t>
+  </si>
+  <si>
+    <t>TUIXYA104370539</t>
+  </si>
+  <si>
+    <t>Normale Belegung eines Doppelzimmers mit zwei Erwachsenen</t>
+  </si>
+  <si>
+    <t>Normale Belegung eines Doppelzimmers, mit einem Kind zusätzlich im Zimmer. Child=1. Da es ein Kind ist, wird nach ChildAdultNr=2 (Normbelegung) gesucht, und das erste Kind kann den Special ChildChildNr=1 anwenden.</t>
+  </si>
+  <si>
+    <t>Normale Belegung eines Doppelzimmers, mit zwei Kinder zusätzlich im Zimmer. Es sind zwei Kinder in dem Zimmer. Es muss für jedes Kind einzeln nach den Specials gesucht werden. Child=1. Für das erste Kind wird nach ChildAdultNr=2 (Normbelegung) gesucht, und ChildChildNr=1. Für das zweite Kind wird nach ChildAdultNr=2 (Normbelegung) gesucht, und ChildChildNr=2. Ansonsten sind die Specials für Kinder in der Logik identisch wie die für Erwachsene. Für die Erwachsene wird nach ChildAdultNr=0 und ChildChildNr=0 gesucht. Rechts die Regeln nur für das letzte Kind. Die Regeln für das erste Kind sind im vorherigen Beispiel dokumentiert wo ChildAdultNr=2 und ChildChildNr=1.</t>
+  </si>
 </sst>
 </file>
 
@@ -859,13 +913,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\ d&quot;, &quot;yy"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1343,52 +1404,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1398,34 +1473,34 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1434,20 +1509,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="43" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="57">
     <cellStyle name="20 % - Akzent1" xfId="17" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1 2" xfId="45"/>
     <cellStyle name="20 % - Akzent2" xfId="21" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2 2" xfId="47"/>
     <cellStyle name="20 % - Akzent3" xfId="25" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3 2" xfId="49"/>
     <cellStyle name="20 % - Akzent4" xfId="29" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4 2" xfId="51"/>
     <cellStyle name="20 % - Akzent5" xfId="33" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5 2" xfId="53"/>
     <cellStyle name="20 % - Akzent6" xfId="37" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6 2" xfId="55"/>
     <cellStyle name="40 % - Akzent1" xfId="18" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1 2" xfId="46"/>
     <cellStyle name="40 % - Akzent2" xfId="22" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2 2" xfId="48"/>
     <cellStyle name="40 % - Akzent3" xfId="26" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3 2" xfId="50"/>
     <cellStyle name="40 % - Akzent4" xfId="30" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4 2" xfId="52"/>
     <cellStyle name="40 % - Akzent5" xfId="34" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5 2" xfId="54"/>
     <cellStyle name="40 % - Akzent6" xfId="38" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6 2" xfId="56"/>
     <cellStyle name="60 % - Akzent1" xfId="19" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent2" xfId="23" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent3" xfId="27" builtinId="40" customBuiltin="1"/>
@@ -1468,9 +1560,11 @@
     <cellStyle name="Gut" xfId="9" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz 2" xfId="42"/>
+    <cellStyle name="Notiz 3" xfId="44"/>
     <cellStyle name="Schlecht" xfId="8" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="40"/>
+    <cellStyle name="Standard 3" xfId="43"/>
     <cellStyle name="Überschrift 1" xfId="13" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="12" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Überschrift 3" xfId="11" builtinId="18" customBuiltin="1"/>
@@ -1481,6 +1575,14 @@
     <cellStyle name="Zelle überprüfen" xfId="2" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="56">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1711,14 +1813,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1919,7 +2013,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:AN992" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:AN989" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <tableColumns count="40">
     <tableColumn id="1" name="ItemType" dataDxfId="39"/>
     <tableColumn id="2" name="Dest" dataDxfId="38"/>
@@ -1932,35 +2026,35 @@
     <tableColumn id="9" name="Inf" dataDxfId="31"/>
     <tableColumn id="10" name="ItemStartDate" dataDxfId="30"/>
     <tableColumn id="11" name="Duration" dataDxfId="29"/>
-    <tableColumn id="12" name="Notes" dataDxfId="28"/>
-    <tableColumn id="13" name="DateFrom" dataDxfId="27"/>
-    <tableColumn id="14" name="DateTo" dataDxfId="26"/>
-    <tableColumn id="15" name="Days" dataDxfId="25"/>
-    <tableColumn id="16" name="DayString" dataDxfId="24"/>
-    <tableColumn id="17" name="RuleDesc" dataDxfId="23"/>
-    <tableColumn id="18" name="PayNights" dataDxfId="22"/>
-    <tableColumn id="19" name="Type" dataDxfId="21"/>
-    <tableColumn id="20" name="EffectiveSpecialDays" dataDxfId="20"/>
-    <tableColumn id="21" name="LastSpOffEndDate" dataDxfId="19"/>
-    <tableColumn id="22" name="RevolvingGroup" dataDxfId="18"/>
-    <tableColumn id="23" name="StartDateRelevant" dataDxfId="17"/>
-    <tableColumn id="24" name="EndDateRelevant" dataDxfId="16"/>
-    <tableColumn id="25" name="DescId" dataDxfId="15"/>
-    <tableColumn id="26" name="DaysBeforeDepartureFrom" dataDxfId="14"/>
-    <tableColumn id="27" name="DaysBeforeDepartureTo" dataDxfId="13"/>
-    <tableColumn id="28" name="DateBeforeDepartureFrom" dataDxfId="12"/>
-    <tableColumn id="29" name="DateBeforeDepartureTo" dataDxfId="11"/>
-    <tableColumn id="30" name="ChildAdultNr" dataDxfId="10"/>
-    <tableColumn id="31" name="ChildChildNr" dataDxfId="9"/>
-    <tableColumn id="32" name="FromDayBase" dataDxfId="8"/>
-    <tableColumn id="33" name="ToDayBase" dataDxfId="7"/>
-    <tableColumn id="34" name="Child" dataDxfId="6"/>
-    <tableColumn id="35" name="Baby" dataDxfId="5"/>
-    <tableColumn id="36" name="RuleType" dataDxfId="4"/>
-    <tableColumn id="37" name="AddAmount" dataDxfId="3"/>
-    <tableColumn id="38" name="ItemSeq" dataDxfId="2"/>
-    <tableColumn id="39" name="ParentSeq" dataDxfId="1"/>
-    <tableColumn id="40" name="SpecialSeq" dataDxfId="0"/>
+    <tableColumn id="12" name="Notes" dataDxfId="0"/>
+    <tableColumn id="13" name="DateFrom" dataDxfId="28"/>
+    <tableColumn id="14" name="DateTo" dataDxfId="27"/>
+    <tableColumn id="15" name="Days" dataDxfId="26"/>
+    <tableColumn id="16" name="DayString" dataDxfId="25"/>
+    <tableColumn id="17" name="RuleDesc" dataDxfId="24"/>
+    <tableColumn id="18" name="PayNights" dataDxfId="23"/>
+    <tableColumn id="19" name="Type" dataDxfId="22"/>
+    <tableColumn id="20" name="EffectiveSpecialDays" dataDxfId="21"/>
+    <tableColumn id="21" name="LastSpOffEndDate" dataDxfId="20"/>
+    <tableColumn id="22" name="RevolvingGroup" dataDxfId="19"/>
+    <tableColumn id="23" name="StartDateRelevant" dataDxfId="18"/>
+    <tableColumn id="24" name="EndDateRelevant" dataDxfId="17"/>
+    <tableColumn id="25" name="DescId" dataDxfId="16"/>
+    <tableColumn id="26" name="DaysBeforeDepartureFrom" dataDxfId="15"/>
+    <tableColumn id="27" name="DaysBeforeDepartureTo" dataDxfId="14"/>
+    <tableColumn id="28" name="DateBeforeDepartureFrom" dataDxfId="13"/>
+    <tableColumn id="29" name="DateBeforeDepartureTo" dataDxfId="12"/>
+    <tableColumn id="30" name="ChildAdultNr" dataDxfId="11"/>
+    <tableColumn id="31" name="ChildChildNr" dataDxfId="10"/>
+    <tableColumn id="32" name="FromDayBase" dataDxfId="9"/>
+    <tableColumn id="33" name="ToDayBase" dataDxfId="8"/>
+    <tableColumn id="34" name="Child" dataDxfId="7"/>
+    <tableColumn id="35" name="Baby" dataDxfId="6"/>
+    <tableColumn id="36" name="RuleType" dataDxfId="5"/>
+    <tableColumn id="37" name="AddAmount" dataDxfId="4"/>
+    <tableColumn id="38" name="ItemSeq" dataDxfId="3"/>
+    <tableColumn id="39" name="ParentSeq" dataDxfId="2"/>
+    <tableColumn id="40" name="SpecialSeq" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2231,8 +2325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L992"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:L95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5288,46 +5382,118 @@
       <c r="L92" s="16"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93" s="15"/>
-      <c r="B93" s="15"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="15"/>
-      <c r="F93" s="15"/>
-      <c r="G93" s="15"/>
-      <c r="H93" s="15"/>
-      <c r="I93" s="15"/>
-      <c r="J93" s="15"/>
-      <c r="K93" s="15"/>
-      <c r="L93" s="16"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A94" s="15"/>
-      <c r="B94" s="15"/>
-      <c r="C94" s="15"/>
-      <c r="D94" s="15"/>
-      <c r="E94" s="15"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="15"/>
-      <c r="H94" s="15"/>
-      <c r="I94" s="15"/>
-      <c r="J94" s="15"/>
-      <c r="K94" s="15"/>
-      <c r="L94" s="16"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" s="15"/>
-      <c r="B95" s="15"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="15"/>
-      <c r="E95" s="15"/>
-      <c r="F95" s="15"/>
-      <c r="G95" s="15"/>
-      <c r="H95" s="15"/>
-      <c r="I95" s="15"/>
-      <c r="J95" s="15"/>
-      <c r="K95" s="15"/>
-      <c r="L95" s="16"/>
+      <c r="A93" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C93" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E93" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="F93" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G93" s="15">
+        <v>2</v>
+      </c>
+      <c r="H93" s="15">
+        <v>0</v>
+      </c>
+      <c r="I93" s="15">
+        <v>0</v>
+      </c>
+      <c r="J93" s="15">
+        <v>42370</v>
+      </c>
+      <c r="K93" s="15">
+        <v>3</v>
+      </c>
+      <c r="L93" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E94" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="F94" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G94" s="15">
+        <v>2</v>
+      </c>
+      <c r="H94" s="15">
+        <v>1</v>
+      </c>
+      <c r="I94" s="15">
+        <v>0</v>
+      </c>
+      <c r="J94" s="15">
+        <v>42370</v>
+      </c>
+      <c r="K94" s="15">
+        <v>3</v>
+      </c>
+      <c r="L94" s="16" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A95" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E95" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="F95" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G95" s="15">
+        <v>2</v>
+      </c>
+      <c r="H95" s="15">
+        <v>2</v>
+      </c>
+      <c r="I95" s="15">
+        <v>0</v>
+      </c>
+      <c r="J95" s="15">
+        <v>42370</v>
+      </c>
+      <c r="K95" s="15">
+        <v>3</v>
+      </c>
+      <c r="L95" s="16" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
@@ -17898,10 +18064,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN91"/>
+  <dimension ref="A1:AN95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:L95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27342,6 +27508,348 @@
         <v>240</v>
       </c>
     </row>
+    <row r="93" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A93" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B93" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="C93" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="D93" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="E93" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F93" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G93" s="17">
+        <v>2</v>
+      </c>
+      <c r="H93" s="17">
+        <v>0</v>
+      </c>
+      <c r="I93" s="17">
+        <v>0</v>
+      </c>
+      <c r="J93" s="18">
+        <v>42370</v>
+      </c>
+      <c r="K93" s="17">
+        <v>3</v>
+      </c>
+      <c r="L93" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="M93" s="18">
+        <v>42370</v>
+      </c>
+      <c r="N93" s="18">
+        <v>42735</v>
+      </c>
+      <c r="O93" s="17">
+        <v>3</v>
+      </c>
+      <c r="P93" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q93" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="R93" s="17">
+        <v>2</v>
+      </c>
+      <c r="S93" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="T93" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="U93" s="18">
+        <v>42735</v>
+      </c>
+      <c r="V93" s="17">
+        <v>0</v>
+      </c>
+      <c r="W93" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="X93" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y93" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z93" s="17"/>
+      <c r="AA93" s="17"/>
+      <c r="AB93" s="17"/>
+      <c r="AC93" s="17"/>
+      <c r="AD93" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE93" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF93" s="17">
+        <v>3</v>
+      </c>
+      <c r="AG93" s="17">
+        <v>3</v>
+      </c>
+      <c r="AH93" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI93" s="17">
+        <v>0</v>
+      </c>
+      <c r="AJ93" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK93" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL93" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="AM93" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="AN93" s="17" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="94" spans="1:40" ht="45" x14ac:dyDescent="0.25">
+      <c r="A94" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="C94" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="D94" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="E94" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F94" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G94" s="17">
+        <v>2</v>
+      </c>
+      <c r="H94" s="17">
+        <v>1</v>
+      </c>
+      <c r="I94" s="17">
+        <v>0</v>
+      </c>
+      <c r="J94" s="18">
+        <v>42370</v>
+      </c>
+      <c r="K94" s="17">
+        <v>3</v>
+      </c>
+      <c r="L94" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="M94" s="18">
+        <v>42370</v>
+      </c>
+      <c r="N94" s="18">
+        <v>42735</v>
+      </c>
+      <c r="O94" s="17">
+        <v>3</v>
+      </c>
+      <c r="P94" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q94" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="R94" s="17">
+        <v>2</v>
+      </c>
+      <c r="S94" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="T94" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="U94" s="18">
+        <v>42735</v>
+      </c>
+      <c r="V94" s="17">
+        <v>0</v>
+      </c>
+      <c r="W94" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="X94" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y94" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z94" s="17"/>
+      <c r="AA94" s="17"/>
+      <c r="AB94" s="17"/>
+      <c r="AC94" s="17"/>
+      <c r="AD94" s="17">
+        <v>2</v>
+      </c>
+      <c r="AE94" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF94" s="17">
+        <v>3</v>
+      </c>
+      <c r="AG94" s="17">
+        <v>3</v>
+      </c>
+      <c r="AH94" s="17">
+        <v>1</v>
+      </c>
+      <c r="AI94" s="17">
+        <v>0</v>
+      </c>
+      <c r="AJ94" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK94" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL94" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="AM94" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="AN94" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="95" spans="1:40" ht="105" x14ac:dyDescent="0.25">
+      <c r="A95" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="D95" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="E95" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G95" s="17">
+        <v>2</v>
+      </c>
+      <c r="H95" s="17">
+        <v>2</v>
+      </c>
+      <c r="I95" s="17">
+        <v>0</v>
+      </c>
+      <c r="J95" s="18">
+        <v>42370</v>
+      </c>
+      <c r="K95" s="17">
+        <v>3</v>
+      </c>
+      <c r="L95" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="M95" s="18">
+        <v>42370</v>
+      </c>
+      <c r="N95" s="18">
+        <v>42735</v>
+      </c>
+      <c r="O95" s="17">
+        <v>3</v>
+      </c>
+      <c r="P95" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q95" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="R95" s="17">
+        <v>2</v>
+      </c>
+      <c r="S95" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="T95" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="U95" s="18">
+        <v>42735</v>
+      </c>
+      <c r="V95" s="17">
+        <v>0</v>
+      </c>
+      <c r="W95" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="X95" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y95" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="Z95" s="17"/>
+      <c r="AA95" s="17"/>
+      <c r="AB95" s="17"/>
+      <c r="AC95" s="17"/>
+      <c r="AD95" s="17">
+        <v>2</v>
+      </c>
+      <c r="AE95" s="17">
+        <v>2</v>
+      </c>
+      <c r="AF95" s="17">
+        <v>3</v>
+      </c>
+      <c r="AG95" s="17">
+        <v>3</v>
+      </c>
+      <c r="AH95" s="17">
+        <v>1</v>
+      </c>
+      <c r="AI95" s="17">
+        <v>0</v>
+      </c>
+      <c r="AJ95" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK95" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL95" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="AM95" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="AN95" s="17" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
zeile 30 Avarge Preis korrigiert
</commit_message>
<xml_diff>
--- a/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
+++ b/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\github\OltSchema\BaseData\HotelExport\SpecialOffers\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
   </bookViews>
@@ -19,12 +14,12 @@
     <sheet name="ToDo" sheetId="5" r:id="rId5"/>
     <sheet name="ResultOld" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="304">
   <si>
     <t>ItemType</t>
   </si>
@@ -980,6 +975,10 @@
     <t xml:space="preserve">(12.05.16-18.05.16) 12.05.16 / 512 
 (19.05.16-25.05.16) 19.05.16 / 519 </t>
   </si>
+  <si>
+    <t xml:space="preserve">(27.01.16-02.02.16) Average / 150 - 11 = 139
+(27.01.16-02.02.16) Average / 150 - 11 = 139 </t>
+  </si>
 </sst>
 </file>
 
@@ -988,13 +987,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\ d&quot;, &quot;yy"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1514,48 +1520,62 @@
   </borders>
   <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1570,22 +1590,8 @@
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1595,34 +1601,34 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1634,71 +1640,74 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="43" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="43" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="43" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="43" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="57" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="57" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="57" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="57" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="57" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="57" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="57" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="57" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="57" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="57" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="57" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="57" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="57" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
@@ -1775,14 +1784,6 @@
     <cellStyle name="Zelle überprüfen" xfId="2" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="112">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2251,6 +2252,14 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2489,86 +2498,86 @@
     <tableColumn id="25" name="DescId" dataDxfId="71" dataCellStyle="Standard 4"/>
     <tableColumn id="26" name="DaysBeforeDepartureFrom" dataDxfId="70" dataCellStyle="Standard 4"/>
     <tableColumn id="27" name="DaysBeforeDepartureTo" dataDxfId="69" dataCellStyle="Standard 4"/>
-    <tableColumn id="28" name="DateBeforeDepartureFrom" dataDxfId="1" dataCellStyle="Standard 4"/>
-    <tableColumn id="29" name="DateBeforeDepartureTo" dataDxfId="0" dataCellStyle="Standard 4"/>
-    <tableColumn id="30" name="ChildAdultNr" dataDxfId="68" dataCellStyle="Standard 4"/>
-    <tableColumn id="31" name="ChildChildNr" dataDxfId="67" dataCellStyle="Standard 4"/>
-    <tableColumn id="32" name="FromDayBase" dataDxfId="66" dataCellStyle="Standard 4"/>
-    <tableColumn id="33" name="ToDayBase" dataDxfId="65" dataCellStyle="Standard 4"/>
-    <tableColumn id="34" name="Child" dataDxfId="64" dataCellStyle="Standard 4"/>
-    <tableColumn id="35" name="Baby" dataDxfId="63" dataCellStyle="Standard 4"/>
-    <tableColumn id="36" name="RuleType" dataDxfId="62" dataCellStyle="Standard 4"/>
-    <tableColumn id="37" name="AddAmount" dataDxfId="61" dataCellStyle="Standard 4"/>
-    <tableColumn id="38" name="ItemSeq" dataDxfId="60" dataCellStyle="Standard 4"/>
-    <tableColumn id="39" name="ParentSeq" dataDxfId="59" dataCellStyle="Standard 4"/>
-    <tableColumn id="40" name="SpecialSeq" dataDxfId="58" dataCellStyle="Standard 4"/>
-    <tableColumn id="41" name="TotalSavings" dataDxfId="57" dataCellStyle="Standard 4"/>
-    <tableColumn id="42" name="TotalPrice" dataDxfId="56" dataCellStyle="Standard 4"/>
-    <tableColumn id="43" name="Spalte1" dataDxfId="55"/>
-    <tableColumn id="44" name="Spalte2" dataDxfId="54"/>
-    <tableColumn id="45" name="Spalte3" dataDxfId="53"/>
-    <tableColumn id="46" name="Spalte4" dataDxfId="52"/>
-    <tableColumn id="47" name="Spalte5" dataDxfId="51"/>
+    <tableColumn id="28" name="DateBeforeDepartureFrom" dataDxfId="68" dataCellStyle="Standard 4"/>
+    <tableColumn id="29" name="DateBeforeDepartureTo" dataDxfId="67" dataCellStyle="Standard 4"/>
+    <tableColumn id="30" name="ChildAdultNr" dataDxfId="66" dataCellStyle="Standard 4"/>
+    <tableColumn id="31" name="ChildChildNr" dataDxfId="65" dataCellStyle="Standard 4"/>
+    <tableColumn id="32" name="FromDayBase" dataDxfId="64" dataCellStyle="Standard 4"/>
+    <tableColumn id="33" name="ToDayBase" dataDxfId="63" dataCellStyle="Standard 4"/>
+    <tableColumn id="34" name="Child" dataDxfId="62" dataCellStyle="Standard 4"/>
+    <tableColumn id="35" name="Baby" dataDxfId="61" dataCellStyle="Standard 4"/>
+    <tableColumn id="36" name="RuleType" dataDxfId="60" dataCellStyle="Standard 4"/>
+    <tableColumn id="37" name="AddAmount" dataDxfId="59" dataCellStyle="Standard 4"/>
+    <tableColumn id="38" name="ItemSeq" dataDxfId="58" dataCellStyle="Standard 4"/>
+    <tableColumn id="39" name="ParentSeq" dataDxfId="57" dataCellStyle="Standard 4"/>
+    <tableColumn id="40" name="SpecialSeq" dataDxfId="56" dataCellStyle="Standard 4"/>
+    <tableColumn id="41" name="TotalSavings" dataDxfId="55" dataCellStyle="Standard 4"/>
+    <tableColumn id="42" name="TotalPrice" dataDxfId="54" dataCellStyle="Standard 4"/>
+    <tableColumn id="43" name="Spalte1" dataDxfId="53"/>
+    <tableColumn id="44" name="Spalte2" dataDxfId="52"/>
+    <tableColumn id="45" name="Spalte3" dataDxfId="51"/>
+    <tableColumn id="46" name="Spalte4" dataDxfId="50"/>
+    <tableColumn id="47" name="Spalte5" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:AN989" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:AN989" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <tableColumns count="40">
-    <tableColumn id="1" name="ItemType" dataDxfId="48"/>
-    <tableColumn id="2" name="Dest" dataDxfId="47"/>
-    <tableColumn id="3" name="ParentCode" dataDxfId="46"/>
-    <tableColumn id="4" name="ItemCode" dataDxfId="45"/>
-    <tableColumn id="5" name="MealCode" dataDxfId="44"/>
-    <tableColumn id="6" name="CurrentDate" dataDxfId="43"/>
-    <tableColumn id="7" name="Adult" dataDxfId="42"/>
-    <tableColumn id="8" name="Chd" dataDxfId="41"/>
-    <tableColumn id="9" name="Inf" dataDxfId="40"/>
-    <tableColumn id="10" name="ItemStartDate" dataDxfId="39"/>
-    <tableColumn id="11" name="Duration" dataDxfId="38"/>
-    <tableColumn id="12" name="Notes" dataDxfId="37"/>
-    <tableColumn id="13" name="DateFrom" dataDxfId="36"/>
-    <tableColumn id="14" name="DateTo" dataDxfId="35"/>
-    <tableColumn id="15" name="Days" dataDxfId="34"/>
-    <tableColumn id="16" name="DayString" dataDxfId="33"/>
-    <tableColumn id="17" name="RuleDesc" dataDxfId="32"/>
-    <tableColumn id="18" name="PayNights" dataDxfId="31"/>
-    <tableColumn id="19" name="Type" dataDxfId="30"/>
-    <tableColumn id="20" name="EffectiveSpecialDays" dataDxfId="29"/>
-    <tableColumn id="21" name="LastSpOffEndDate" dataDxfId="28"/>
-    <tableColumn id="22" name="RevolvingGroup" dataDxfId="27"/>
-    <tableColumn id="23" name="StartDateRelevant" dataDxfId="26"/>
-    <tableColumn id="24" name="EndDateRelevant" dataDxfId="25"/>
-    <tableColumn id="25" name="DescId" dataDxfId="24"/>
-    <tableColumn id="26" name="DaysBeforeDepartureFrom" dataDxfId="23"/>
-    <tableColumn id="27" name="DaysBeforeDepartureTo" dataDxfId="22"/>
-    <tableColumn id="28" name="DateBeforeDepartureFrom" dataDxfId="21"/>
-    <tableColumn id="29" name="DateBeforeDepartureTo" dataDxfId="20"/>
-    <tableColumn id="30" name="ChildAdultNr" dataDxfId="19"/>
-    <tableColumn id="31" name="ChildChildNr" dataDxfId="18"/>
-    <tableColumn id="32" name="FromDayBase" dataDxfId="17"/>
-    <tableColumn id="33" name="ToDayBase" dataDxfId="16"/>
-    <tableColumn id="34" name="Child" dataDxfId="15"/>
-    <tableColumn id="35" name="Baby" dataDxfId="14"/>
-    <tableColumn id="36" name="RuleType" dataDxfId="13"/>
-    <tableColumn id="37" name="AddAmount" dataDxfId="12"/>
-    <tableColumn id="38" name="ItemSeq" dataDxfId="11"/>
-    <tableColumn id="39" name="ParentSeq" dataDxfId="10"/>
-    <tableColumn id="40" name="SpecialSeq" dataDxfId="9"/>
+    <tableColumn id="1" name="ItemType" dataDxfId="46"/>
+    <tableColumn id="2" name="Dest" dataDxfId="45"/>
+    <tableColumn id="3" name="ParentCode" dataDxfId="44"/>
+    <tableColumn id="4" name="ItemCode" dataDxfId="43"/>
+    <tableColumn id="5" name="MealCode" dataDxfId="42"/>
+    <tableColumn id="6" name="CurrentDate" dataDxfId="41"/>
+    <tableColumn id="7" name="Adult" dataDxfId="40"/>
+    <tableColumn id="8" name="Chd" dataDxfId="39"/>
+    <tableColumn id="9" name="Inf" dataDxfId="38"/>
+    <tableColumn id="10" name="ItemStartDate" dataDxfId="37"/>
+    <tableColumn id="11" name="Duration" dataDxfId="36"/>
+    <tableColumn id="12" name="Notes" dataDxfId="35"/>
+    <tableColumn id="13" name="DateFrom" dataDxfId="34"/>
+    <tableColumn id="14" name="DateTo" dataDxfId="33"/>
+    <tableColumn id="15" name="Days" dataDxfId="32"/>
+    <tableColumn id="16" name="DayString" dataDxfId="31"/>
+    <tableColumn id="17" name="RuleDesc" dataDxfId="30"/>
+    <tableColumn id="18" name="PayNights" dataDxfId="29"/>
+    <tableColumn id="19" name="Type" dataDxfId="28"/>
+    <tableColumn id="20" name="EffectiveSpecialDays" dataDxfId="27"/>
+    <tableColumn id="21" name="LastSpOffEndDate" dataDxfId="26"/>
+    <tableColumn id="22" name="RevolvingGroup" dataDxfId="25"/>
+    <tableColumn id="23" name="StartDateRelevant" dataDxfId="24"/>
+    <tableColumn id="24" name="EndDateRelevant" dataDxfId="23"/>
+    <tableColumn id="25" name="DescId" dataDxfId="22"/>
+    <tableColumn id="26" name="DaysBeforeDepartureFrom" dataDxfId="21"/>
+    <tableColumn id="27" name="DaysBeforeDepartureTo" dataDxfId="20"/>
+    <tableColumn id="28" name="DateBeforeDepartureFrom" dataDxfId="19"/>
+    <tableColumn id="29" name="DateBeforeDepartureTo" dataDxfId="18"/>
+    <tableColumn id="30" name="ChildAdultNr" dataDxfId="17"/>
+    <tableColumn id="31" name="ChildChildNr" dataDxfId="16"/>
+    <tableColumn id="32" name="FromDayBase" dataDxfId="15"/>
+    <tableColumn id="33" name="ToDayBase" dataDxfId="14"/>
+    <tableColumn id="34" name="Child" dataDxfId="13"/>
+    <tableColumn id="35" name="Baby" dataDxfId="12"/>
+    <tableColumn id="36" name="RuleType" dataDxfId="11"/>
+    <tableColumn id="37" name="AddAmount" dataDxfId="10"/>
+    <tableColumn id="38" name="ItemSeq" dataDxfId="9"/>
+    <tableColumn id="39" name="ParentSeq" dataDxfId="8"/>
+    <tableColumn id="40" name="SpecialSeq" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="AO1:AQ1048576" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="AO1:AQ1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
   <autoFilter ref="AO1:AQ1048576"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="TotalSavings" dataDxfId="4"/>
-    <tableColumn id="2" name="TotalPrice" dataDxfId="3"/>
-    <tableColumn id="3" name="Spalte1" dataDxfId="2"/>
+    <tableColumn id="1" name="TotalSavings" dataDxfId="2"/>
+    <tableColumn id="2" name="TotalPrice" dataDxfId="1"/>
+    <tableColumn id="3" name="Spalte1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2829,7 +2838,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -18984,8 +18993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC87" sqref="AC1:AC1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AB28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AQ30" sqref="AQ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22485,8 +22494,8 @@
       <c r="S30" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="T30" s="27" t="s">
-        <v>87</v>
+      <c r="T30" s="40" t="s">
+        <v>303</v>
       </c>
       <c r="U30" s="28">
         <v>42402</v>
@@ -22545,10 +22554,10 @@
         <v>133</v>
       </c>
       <c r="AO30" s="26">
-        <v>-233</v>
+        <v>-278</v>
       </c>
       <c r="AP30" s="26">
-        <v>815</v>
+        <v>770</v>
       </c>
     </row>
     <row r="32" spans="1:42" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Avarage Preise auf dezimal geändert
</commit_message>
<xml_diff>
--- a/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
+++ b/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3505" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3523" uniqueCount="312">
   <si>
     <t>ItemType</t>
   </si>
@@ -982,10 +982,6 @@
     <t>7</t>
   </si>
   <si>
-    <t xml:space="preserve">(27.01.16-02.02.16) Average / 149.71 - 11 = 138 
-(27.01.16-02.02.16) Average / 149.71 - 11 = 138 </t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -993,6 +989,21 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>MinDays, MaxDays,MinAmount,MaxAmount,Average in Verbindung mit StartDateRelevant. Dieses Beispiel zeigt die Anwendung vom Average. Die effektiven PerDayPrices sind vom 23JAN bis 29JAN, es wird ein Durchschnitt der Preise gemacht, und da die Duration 7 Tage ist, und PayNights=5 wird der Average-Betrag zwei Mal abgezogen. Wichtig hier: wenn es ein Days=13 DayString=7,6 gibt, dann muss jede 7-Tage-Gruppe für sich betrachtet werden. Es darf kein Average aller Tage 13 berechnet werden, sondern die ersten 7 Tage Gruppe und die zweite 6 Tage Gruppe müssen unabhängig voneinander betrachtet werden.</t>
+  </si>
+  <si>
+    <t>MinDays, MaxDays,MinAmount,MaxAmount,Average in Verbindung mit StartDateRelevant. Dieses Beispiel zeigt die Anwendung vom Average. Die effektiven PerDayPrices sind vom 23JAN bis 29JAN, es wird ein Durchschnitt der Preise gemacht, und da die Duration 7 Tage ist, und PayNights=5 wird der Average-Betrag zwei Mal abgezogen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(27.01.16-02.02.16) Average / 149.71 - 11 = 138.71 
+(27.01.16-02.02.16) Average / 149.71 - 11 = 138.71 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(27.01.16-02.02.16) Average / 149.71 - 11 = 138.71 
+(27.01.16-02.02.16) Average / 149.71 - 11 = 138.71 
+(03.02.16-08.02.16) Average / 205.50 - 11 = 194.50 </t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1624,7 @@
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1729,9 +1740,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="57" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="57" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="57" applyFill="1" applyAlignment="1">
@@ -1751,6 +1759,12 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="57" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="57" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
@@ -2511,8 +2525,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A1:AU108" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
-  <autoFilter ref="A1:AU108"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A1:AU110" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+  <autoFilter ref="A1:AU110"/>
   <tableColumns count="47">
     <tableColumn id="1" name="ItemType" dataDxfId="95" dataCellStyle="Standard 4"/>
     <tableColumn id="2" name="Dest" dataDxfId="94" dataCellStyle="Standard 4"/>
@@ -2881,7 +2895,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -19034,10 +19048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU108"/>
+  <dimension ref="A1:AU110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T90" sqref="T90"/>
+    <sheetView tabSelected="1" topLeftCell="O25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19232,7 +19246,7 @@
       </c>
     </row>
     <row r="2" spans="1:47" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -22479,7 +22493,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="30" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>36</v>
       </c>
@@ -22513,8 +22527,8 @@
       <c r="K30" s="35">
         <v>7</v>
       </c>
-      <c r="L30" s="27" t="s">
-        <v>171</v>
+      <c r="L30" s="47" t="s">
+        <v>309</v>
       </c>
       <c r="M30" s="28">
         <v>42396</v>
@@ -22537,8 +22551,8 @@
       <c r="S30" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="T30" s="40" t="s">
-        <v>305</v>
+      <c r="T30" s="47" t="s">
+        <v>310</v>
       </c>
       <c r="U30" s="28">
         <v>42402</v>
@@ -23754,7 +23768,7 @@
         <v>5</v>
       </c>
       <c r="P42" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q42" s="25" t="s">
         <v>140</v>
@@ -23874,7 +23888,7 @@
         <v>5</v>
       </c>
       <c r="P43" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q43" s="25" t="s">
         <v>140</v>
@@ -24234,7 +24248,7 @@
         <v>5</v>
       </c>
       <c r="P47" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q47" s="25" t="s">
         <v>140</v>
@@ -24354,7 +24368,7 @@
         <v>5</v>
       </c>
       <c r="P48" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q48" s="25" t="s">
         <v>140</v>
@@ -25182,7 +25196,7 @@
         <v>5</v>
       </c>
       <c r="P58" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q58" s="25" t="s">
         <v>140</v>
@@ -25554,7 +25568,7 @@
         <v>5</v>
       </c>
       <c r="P62" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q62" s="25" t="s">
         <v>140</v>
@@ -25802,7 +25816,7 @@
         <v>5</v>
       </c>
       <c r="P65" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q65" s="25" t="s">
         <v>140</v>
@@ -25922,7 +25936,7 @@
         <v>5</v>
       </c>
       <c r="P66" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q66" s="25" t="s">
         <v>140</v>
@@ -26042,7 +26056,7 @@
         <v>5</v>
       </c>
       <c r="P67" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q67" s="25" t="s">
         <v>140</v>
@@ -26162,7 +26176,7 @@
         <v>5</v>
       </c>
       <c r="P68" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q68" s="25" t="s">
         <v>140</v>
@@ -26282,7 +26296,7 @@
         <v>5</v>
       </c>
       <c r="P69" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q69" s="25" t="s">
         <v>140</v>
@@ -27056,7 +27070,7 @@
         <v>5</v>
       </c>
       <c r="P77" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q77" s="25" t="s">
         <v>140</v>
@@ -28316,7 +28330,7 @@
       </c>
     </row>
     <row r="90" spans="1:42" ht="135" x14ac:dyDescent="0.25">
-      <c r="A90" s="41" t="s">
+      <c r="A90" s="40" t="s">
         <v>36</v>
       </c>
       <c r="B90" s="25" t="s">
@@ -28362,7 +28376,7 @@
         <v>21</v>
       </c>
       <c r="P90" s="38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q90" s="25" t="s">
         <v>234</v>
@@ -28576,7 +28590,7 @@
         <v>3</v>
       </c>
       <c r="P93" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q93" s="25" t="s">
         <v>265</v>
@@ -28696,7 +28710,7 @@
         <v>3</v>
       </c>
       <c r="P94" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q94" s="25" t="s">
         <v>265</v>
@@ -28816,7 +28830,7 @@
         <v>3</v>
       </c>
       <c r="P95" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q95" s="25" t="s">
         <v>265</v>
@@ -28890,1186 +28904,1354 @@
       </c>
     </row>
     <row r="96" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A96" s="42"/>
-      <c r="B96" s="42"/>
-      <c r="C96" s="42"/>
-      <c r="D96" s="42"/>
-      <c r="E96" s="42"/>
-      <c r="F96" s="43"/>
-      <c r="G96" s="44"/>
-      <c r="H96" s="44"/>
-      <c r="I96" s="44"/>
-      <c r="J96" s="43"/>
-      <c r="K96" s="44"/>
-      <c r="L96" s="45"/>
-      <c r="M96" s="43"/>
-      <c r="N96" s="43"/>
-      <c r="O96" s="44"/>
-      <c r="P96" s="46"/>
-      <c r="Q96" s="42"/>
-      <c r="R96" s="44"/>
-      <c r="S96" s="42"/>
-      <c r="T96" s="42"/>
-      <c r="U96" s="43"/>
-      <c r="V96" s="44"/>
-      <c r="W96" s="42"/>
-      <c r="X96" s="42"/>
-      <c r="Y96" s="45"/>
-      <c r="Z96" s="44"/>
-      <c r="AA96" s="44"/>
-      <c r="AB96" s="43"/>
-      <c r="AC96" s="43"/>
-      <c r="AD96" s="44"/>
-      <c r="AE96" s="44"/>
-      <c r="AF96" s="44"/>
-      <c r="AG96" s="44"/>
-      <c r="AH96" s="44"/>
-      <c r="AI96" s="44"/>
-      <c r="AJ96" s="42"/>
-      <c r="AK96" s="47"/>
-      <c r="AL96" s="42"/>
-      <c r="AM96" s="42"/>
-      <c r="AN96" s="42"/>
-      <c r="AO96" s="47"/>
-      <c r="AP96" s="47"/>
+      <c r="A96" s="41"/>
+      <c r="B96" s="41"/>
+      <c r="C96" s="41"/>
+      <c r="D96" s="41"/>
+      <c r="E96" s="41"/>
+      <c r="F96" s="42"/>
+      <c r="G96" s="43"/>
+      <c r="H96" s="43"/>
+      <c r="I96" s="43"/>
+      <c r="J96" s="42"/>
+      <c r="K96" s="43"/>
+      <c r="L96" s="44"/>
+      <c r="M96" s="42"/>
+      <c r="N96" s="42"/>
+      <c r="O96" s="43"/>
+      <c r="P96" s="45"/>
+      <c r="Q96" s="41"/>
+      <c r="R96" s="43"/>
+      <c r="S96" s="41"/>
+      <c r="T96" s="41"/>
+      <c r="U96" s="42"/>
+      <c r="V96" s="43"/>
+      <c r="W96" s="41"/>
+      <c r="X96" s="41"/>
+      <c r="Y96" s="44"/>
+      <c r="Z96" s="43"/>
+      <c r="AA96" s="43"/>
+      <c r="AB96" s="42"/>
+      <c r="AC96" s="42"/>
+      <c r="AD96" s="43"/>
+      <c r="AE96" s="43"/>
+      <c r="AF96" s="43"/>
+      <c r="AG96" s="43"/>
+      <c r="AH96" s="43"/>
+      <c r="AI96" s="43"/>
+      <c r="AJ96" s="41"/>
+      <c r="AK96" s="46"/>
+      <c r="AL96" s="41"/>
+      <c r="AM96" s="41"/>
+      <c r="AN96" s="41"/>
+      <c r="AO96" s="46"/>
+      <c r="AP96" s="46"/>
     </row>
     <row r="97" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A97" s="42" t="s">
+      <c r="A97" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B97" s="42" t="s">
+      <c r="B97" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C97" s="42" t="s">
+      <c r="C97" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="D97" s="42" t="s">
+      <c r="D97" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="E97" s="42" t="s">
+      <c r="E97" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F97" s="43" t="s">
+      <c r="F97" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G97" s="44">
+      <c r="G97" s="43">
         <v>1</v>
       </c>
-      <c r="H97" s="44">
-        <v>0</v>
-      </c>
-      <c r="I97" s="44">
-        <v>0</v>
-      </c>
-      <c r="J97" s="43">
+      <c r="H97" s="43">
+        <v>0</v>
+      </c>
+      <c r="I97" s="43">
+        <v>0</v>
+      </c>
+      <c r="J97" s="42">
         <v>42430</v>
       </c>
-      <c r="K97" s="44">
+      <c r="K97" s="43">
         <v>30</v>
       </c>
-      <c r="L97" s="45"/>
-      <c r="M97" s="43">
+      <c r="L97" s="44"/>
+      <c r="M97" s="42">
         <v>42430</v>
       </c>
-      <c r="N97" s="43">
+      <c r="N97" s="42">
         <v>42434</v>
       </c>
-      <c r="O97" s="44">
+      <c r="O97" s="43">
         <v>4</v>
       </c>
-      <c r="P97" s="46" t="s">
+      <c r="P97" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="Q97" s="42" t="s">
+      <c r="Q97" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="R97" s="44">
+      <c r="R97" s="43">
         <v>3</v>
       </c>
-      <c r="S97" s="42" t="s">
+      <c r="S97" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="T97" s="42" t="s">
+      <c r="T97" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="U97" s="43">
+      <c r="U97" s="42">
         <v>42434</v>
       </c>
-      <c r="V97" s="44">
+      <c r="V97" s="43">
         <v>3</v>
       </c>
-      <c r="W97" s="42" t="s">
+      <c r="W97" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="X97" s="42" t="s">
+      <c r="X97" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="Y97" s="45" t="s">
+      <c r="Y97" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="Z97" s="44"/>
-      <c r="AA97" s="44"/>
-      <c r="AB97" s="43"/>
-      <c r="AC97" s="43"/>
-      <c r="AD97" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE97" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF97" s="44">
+      <c r="Z97" s="43"/>
+      <c r="AA97" s="43"/>
+      <c r="AB97" s="42"/>
+      <c r="AC97" s="42"/>
+      <c r="AD97" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE97" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF97" s="43">
         <v>4</v>
       </c>
-      <c r="AG97" s="44">
+      <c r="AG97" s="43">
         <v>4</v>
       </c>
-      <c r="AH97" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI97" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ97" s="42" t="s">
+      <c r="AH97" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI97" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ97" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="AK97" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL97" s="42" t="s">
+      <c r="AK97" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL97" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM97" s="42" t="s">
+      <c r="AM97" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN97" s="42" t="s">
+      <c r="AN97" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="AO97" s="47">
+      <c r="AO97" s="46">
         <v>-932</v>
       </c>
-      <c r="AP97" s="47">
+      <c r="AP97" s="46">
         <v>8533</v>
       </c>
     </row>
     <row r="98" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A98" s="42" t="s">
+      <c r="A98" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B98" s="42"/>
-      <c r="C98" s="42"/>
-      <c r="D98" s="42"/>
-      <c r="E98" s="42"/>
-      <c r="F98" s="43"/>
-      <c r="G98" s="44"/>
-      <c r="H98" s="44"/>
-      <c r="I98" s="44"/>
-      <c r="J98" s="43"/>
-      <c r="K98" s="44"/>
-      <c r="L98" s="45"/>
-      <c r="M98" s="43">
+      <c r="B98" s="41"/>
+      <c r="C98" s="41"/>
+      <c r="D98" s="41"/>
+      <c r="E98" s="41"/>
+      <c r="F98" s="42"/>
+      <c r="G98" s="43"/>
+      <c r="H98" s="43"/>
+      <c r="I98" s="43"/>
+      <c r="J98" s="42"/>
+      <c r="K98" s="43"/>
+      <c r="L98" s="44"/>
+      <c r="M98" s="42">
         <v>42436</v>
       </c>
-      <c r="N98" s="43">
+      <c r="N98" s="42">
         <v>42441</v>
       </c>
-      <c r="O98" s="44">
+      <c r="O98" s="43">
         <v>4</v>
       </c>
-      <c r="P98" s="46" t="s">
+      <c r="P98" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="Q98" s="42" t="s">
+      <c r="Q98" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="R98" s="44">
+      <c r="R98" s="43">
         <v>3</v>
       </c>
-      <c r="S98" s="42" t="s">
+      <c r="S98" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="T98" s="42" t="s">
+      <c r="T98" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="U98" s="43">
+      <c r="U98" s="42">
         <v>42441</v>
       </c>
-      <c r="V98" s="44">
+      <c r="V98" s="43">
         <v>3</v>
       </c>
-      <c r="W98" s="42" t="s">
+      <c r="W98" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="X98" s="42" t="s">
+      <c r="X98" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="Y98" s="45" t="s">
+      <c r="Y98" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="Z98" s="44"/>
-      <c r="AA98" s="44"/>
-      <c r="AB98" s="43"/>
-      <c r="AC98" s="43"/>
-      <c r="AD98" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE98" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF98" s="44">
+      <c r="Z98" s="43"/>
+      <c r="AA98" s="43"/>
+      <c r="AB98" s="42"/>
+      <c r="AC98" s="42"/>
+      <c r="AD98" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE98" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF98" s="43">
         <v>4</v>
       </c>
-      <c r="AG98" s="44">
+      <c r="AG98" s="43">
         <v>4</v>
       </c>
-      <c r="AH98" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI98" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ98" s="42" t="s">
+      <c r="AH98" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI98" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ98" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="AK98" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL98" s="42" t="s">
+      <c r="AK98" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL98" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM98" s="42" t="s">
+      <c r="AM98" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN98" s="42" t="s">
+      <c r="AN98" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="AO98" s="47"/>
-      <c r="AP98" s="47"/>
+      <c r="AO98" s="46"/>
+      <c r="AP98" s="46"/>
     </row>
     <row r="99" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A99" s="42" t="s">
+      <c r="A99" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B99" s="42"/>
-      <c r="C99" s="42"/>
-      <c r="D99" s="42"/>
-      <c r="E99" s="42"/>
-      <c r="F99" s="43"/>
-      <c r="G99" s="44"/>
-      <c r="H99" s="44"/>
-      <c r="I99" s="44"/>
-      <c r="J99" s="43"/>
-      <c r="K99" s="44"/>
-      <c r="L99" s="45"/>
-      <c r="M99" s="43">
+      <c r="B99" s="41"/>
+      <c r="C99" s="41"/>
+      <c r="D99" s="41"/>
+      <c r="E99" s="41"/>
+      <c r="F99" s="42"/>
+      <c r="G99" s="43"/>
+      <c r="H99" s="43"/>
+      <c r="I99" s="43"/>
+      <c r="J99" s="42"/>
+      <c r="K99" s="43"/>
+      <c r="L99" s="44"/>
+      <c r="M99" s="42">
         <v>42443</v>
       </c>
-      <c r="N99" s="43">
+      <c r="N99" s="42">
         <v>42449</v>
       </c>
-      <c r="O99" s="44">
+      <c r="O99" s="43">
         <v>5</v>
       </c>
-      <c r="P99" s="46" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q99" s="42" t="s">
+      <c r="P99" s="45" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q99" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="R99" s="44">
+      <c r="R99" s="43">
         <v>4</v>
       </c>
-      <c r="S99" s="42" t="s">
+      <c r="S99" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="T99" s="42" t="s">
+      <c r="T99" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="U99" s="43">
+      <c r="U99" s="42">
         <v>42449</v>
       </c>
-      <c r="V99" s="44">
-        <v>0</v>
-      </c>
-      <c r="W99" s="42" t="s">
+      <c r="V99" s="43">
+        <v>0</v>
+      </c>
+      <c r="W99" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="X99" s="42" t="s">
+      <c r="X99" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="Y99" s="45" t="s">
+      <c r="Y99" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="Z99" s="44">
+      <c r="Z99" s="43">
         <v>999</v>
       </c>
-      <c r="AA99" s="44">
+      <c r="AA99" s="43">
         <v>60</v>
       </c>
-      <c r="AB99" s="43"/>
-      <c r="AC99" s="43"/>
-      <c r="AD99" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE99" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF99" s="44">
+      <c r="AB99" s="42"/>
+      <c r="AC99" s="42"/>
+      <c r="AD99" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE99" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF99" s="43">
         <v>5</v>
       </c>
-      <c r="AG99" s="44">
+      <c r="AG99" s="43">
         <v>5</v>
       </c>
-      <c r="AH99" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI99" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ99" s="42" t="s">
+      <c r="AH99" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI99" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ99" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="AK99" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL99" s="42" t="s">
+      <c r="AK99" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL99" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM99" s="42" t="s">
+      <c r="AM99" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN99" s="42" t="s">
+      <c r="AN99" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="AO99" s="47"/>
-      <c r="AP99" s="47"/>
+      <c r="AO99" s="46"/>
+      <c r="AP99" s="46"/>
     </row>
     <row r="100" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A100" s="42"/>
-      <c r="B100" s="42"/>
-      <c r="C100" s="42"/>
-      <c r="D100" s="42"/>
-      <c r="E100" s="42"/>
-      <c r="F100" s="43"/>
-      <c r="G100" s="44"/>
-      <c r="H100" s="44"/>
-      <c r="I100" s="44"/>
-      <c r="J100" s="43"/>
-      <c r="K100" s="44"/>
-      <c r="L100" s="45"/>
-      <c r="M100" s="43"/>
-      <c r="N100" s="43"/>
-      <c r="O100" s="44"/>
-      <c r="P100" s="46"/>
-      <c r="Q100" s="42"/>
-      <c r="R100" s="44"/>
-      <c r="S100" s="42"/>
-      <c r="T100" s="42"/>
-      <c r="U100" s="43"/>
-      <c r="V100" s="44"/>
-      <c r="W100" s="42"/>
-      <c r="X100" s="42"/>
-      <c r="Y100" s="45"/>
-      <c r="Z100" s="44"/>
-      <c r="AA100" s="44"/>
-      <c r="AB100" s="43"/>
-      <c r="AC100" s="43"/>
-      <c r="AD100" s="44"/>
-      <c r="AE100" s="44"/>
-      <c r="AF100" s="44"/>
-      <c r="AG100" s="44"/>
-      <c r="AH100" s="44"/>
-      <c r="AI100" s="44"/>
-      <c r="AJ100" s="42"/>
-      <c r="AK100" s="47"/>
-      <c r="AL100" s="42"/>
-      <c r="AM100" s="42"/>
-      <c r="AN100" s="42"/>
-      <c r="AO100" s="47"/>
-      <c r="AP100" s="47"/>
+      <c r="A100" s="41"/>
+      <c r="B100" s="41"/>
+      <c r="C100" s="41"/>
+      <c r="D100" s="41"/>
+      <c r="E100" s="41"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="43"/>
+      <c r="H100" s="43"/>
+      <c r="I100" s="43"/>
+      <c r="J100" s="42"/>
+      <c r="K100" s="43"/>
+      <c r="L100" s="44"/>
+      <c r="M100" s="42"/>
+      <c r="N100" s="42"/>
+      <c r="O100" s="43"/>
+      <c r="P100" s="45"/>
+      <c r="Q100" s="41"/>
+      <c r="R100" s="43"/>
+      <c r="S100" s="41"/>
+      <c r="T100" s="41"/>
+      <c r="U100" s="42"/>
+      <c r="V100" s="43"/>
+      <c r="W100" s="41"/>
+      <c r="X100" s="41"/>
+      <c r="Y100" s="44"/>
+      <c r="Z100" s="43"/>
+      <c r="AA100" s="43"/>
+      <c r="AB100" s="42"/>
+      <c r="AC100" s="42"/>
+      <c r="AD100" s="43"/>
+      <c r="AE100" s="43"/>
+      <c r="AF100" s="43"/>
+      <c r="AG100" s="43"/>
+      <c r="AH100" s="43"/>
+      <c r="AI100" s="43"/>
+      <c r="AJ100" s="41"/>
+      <c r="AK100" s="46"/>
+      <c r="AL100" s="41"/>
+      <c r="AM100" s="41"/>
+      <c r="AN100" s="41"/>
+      <c r="AO100" s="46"/>
+      <c r="AP100" s="46"/>
     </row>
     <row r="101" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A101" s="42" t="s">
+      <c r="A101" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B101" s="42" t="s">
+      <c r="B101" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C101" s="42" t="s">
+      <c r="C101" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="D101" s="42" t="s">
+      <c r="D101" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="E101" s="42" t="s">
+      <c r="E101" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F101" s="43" t="s">
+      <c r="F101" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G101" s="44">
+      <c r="G101" s="43">
         <v>1</v>
       </c>
-      <c r="H101" s="44">
-        <v>0</v>
-      </c>
-      <c r="I101" s="44">
-        <v>0</v>
-      </c>
-      <c r="J101" s="43">
+      <c r="H101" s="43">
+        <v>0</v>
+      </c>
+      <c r="I101" s="43">
+        <v>0</v>
+      </c>
+      <c r="J101" s="42">
         <v>42430</v>
       </c>
-      <c r="K101" s="44">
+      <c r="K101" s="43">
         <v>91</v>
       </c>
-      <c r="L101" s="45"/>
-      <c r="M101" s="43">
+      <c r="L101" s="44"/>
+      <c r="M101" s="42">
         <v>42430</v>
       </c>
-      <c r="N101" s="43">
+      <c r="N101" s="42">
         <v>42434</v>
       </c>
-      <c r="O101" s="44">
+      <c r="O101" s="43">
         <v>4</v>
       </c>
-      <c r="P101" s="46" t="s">
+      <c r="P101" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="Q101" s="42" t="s">
+      <c r="Q101" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="R101" s="44">
+      <c r="R101" s="43">
         <v>3</v>
       </c>
-      <c r="S101" s="42" t="s">
+      <c r="S101" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="T101" s="42" t="s">
+      <c r="T101" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="U101" s="43">
+      <c r="U101" s="42">
         <v>42434</v>
       </c>
-      <c r="V101" s="44">
+      <c r="V101" s="43">
         <v>3</v>
       </c>
-      <c r="W101" s="42" t="s">
+      <c r="W101" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="X101" s="42" t="s">
+      <c r="X101" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="Y101" s="45" t="s">
+      <c r="Y101" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="Z101" s="44"/>
-      <c r="AA101" s="44"/>
-      <c r="AB101" s="43"/>
-      <c r="AC101" s="43"/>
-      <c r="AD101" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE101" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF101" s="44">
+      <c r="Z101" s="43"/>
+      <c r="AA101" s="43"/>
+      <c r="AB101" s="42"/>
+      <c r="AC101" s="42"/>
+      <c r="AD101" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE101" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF101" s="43">
         <v>4</v>
       </c>
-      <c r="AG101" s="44">
+      <c r="AG101" s="43">
         <v>4</v>
       </c>
-      <c r="AH101" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI101" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ101" s="42" t="s">
+      <c r="AH101" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI101" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ101" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="AK101" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL101" s="42" t="s">
+      <c r="AK101" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL101" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM101" s="42" t="s">
+      <c r="AM101" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN101" s="42" t="s">
+      <c r="AN101" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="AO101" s="47">
+      <c r="AO101" s="46">
         <v>-3900</v>
       </c>
-      <c r="AP101" s="47">
+      <c r="AP101" s="46">
         <v>33826</v>
       </c>
     </row>
     <row r="102" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A102" s="42" t="s">
+      <c r="A102" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B102" s="42"/>
-      <c r="C102" s="42"/>
-      <c r="D102" s="42"/>
-      <c r="E102" s="42"/>
-      <c r="F102" s="43"/>
-      <c r="G102" s="44"/>
-      <c r="H102" s="44"/>
-      <c r="I102" s="44"/>
-      <c r="J102" s="43"/>
-      <c r="K102" s="44"/>
-      <c r="L102" s="45"/>
-      <c r="M102" s="43">
+      <c r="B102" s="41"/>
+      <c r="C102" s="41"/>
+      <c r="D102" s="41"/>
+      <c r="E102" s="41"/>
+      <c r="F102" s="42"/>
+      <c r="G102" s="43"/>
+      <c r="H102" s="43"/>
+      <c r="I102" s="43"/>
+      <c r="J102" s="42"/>
+      <c r="K102" s="43"/>
+      <c r="L102" s="44"/>
+      <c r="M102" s="42">
         <v>42436</v>
       </c>
-      <c r="N102" s="43">
+      <c r="N102" s="42">
         <v>42441</v>
       </c>
-      <c r="O102" s="44">
+      <c r="O102" s="43">
         <v>4</v>
       </c>
-      <c r="P102" s="46" t="s">
+      <c r="P102" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="Q102" s="42" t="s">
+      <c r="Q102" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="R102" s="44">
+      <c r="R102" s="43">
         <v>3</v>
       </c>
-      <c r="S102" s="42" t="s">
+      <c r="S102" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="T102" s="42" t="s">
+      <c r="T102" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="U102" s="43">
+      <c r="U102" s="42">
         <v>42441</v>
       </c>
-      <c r="V102" s="44">
+      <c r="V102" s="43">
         <v>3</v>
       </c>
-      <c r="W102" s="42" t="s">
+      <c r="W102" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="X102" s="42" t="s">
+      <c r="X102" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="Y102" s="45" t="s">
+      <c r="Y102" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="Z102" s="44"/>
-      <c r="AA102" s="44"/>
-      <c r="AB102" s="43"/>
-      <c r="AC102" s="43"/>
-      <c r="AD102" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE102" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF102" s="44">
+      <c r="Z102" s="43"/>
+      <c r="AA102" s="43"/>
+      <c r="AB102" s="42"/>
+      <c r="AC102" s="42"/>
+      <c r="AD102" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE102" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF102" s="43">
         <v>4</v>
       </c>
-      <c r="AG102" s="44">
+      <c r="AG102" s="43">
         <v>4</v>
       </c>
-      <c r="AH102" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI102" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ102" s="42" t="s">
+      <c r="AH102" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI102" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ102" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="AK102" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL102" s="42" t="s">
+      <c r="AK102" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL102" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM102" s="42" t="s">
+      <c r="AM102" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN102" s="42" t="s">
+      <c r="AN102" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="AO102" s="47"/>
-      <c r="AP102" s="47"/>
+      <c r="AO102" s="46"/>
+      <c r="AP102" s="46"/>
     </row>
     <row r="103" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A103" s="42" t="s">
+      <c r="A103" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B103" s="42"/>
-      <c r="C103" s="42"/>
-      <c r="D103" s="42"/>
-      <c r="E103" s="42"/>
-      <c r="F103" s="43"/>
-      <c r="G103" s="44"/>
-      <c r="H103" s="44"/>
-      <c r="I103" s="44"/>
-      <c r="J103" s="43"/>
-      <c r="K103" s="44"/>
-      <c r="L103" s="45"/>
-      <c r="M103" s="43">
+      <c r="B103" s="41"/>
+      <c r="C103" s="41"/>
+      <c r="D103" s="41"/>
+      <c r="E103" s="41"/>
+      <c r="F103" s="42"/>
+      <c r="G103" s="43"/>
+      <c r="H103" s="43"/>
+      <c r="I103" s="43"/>
+      <c r="J103" s="42"/>
+      <c r="K103" s="43"/>
+      <c r="L103" s="44"/>
+      <c r="M103" s="42">
         <v>42443</v>
       </c>
-      <c r="N103" s="43">
+      <c r="N103" s="42">
         <v>42449</v>
       </c>
-      <c r="O103" s="44">
+      <c r="O103" s="43">
         <v>5</v>
       </c>
-      <c r="P103" s="46" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q103" s="42" t="s">
+      <c r="P103" s="45" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q103" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="R103" s="44">
+      <c r="R103" s="43">
         <v>4</v>
       </c>
-      <c r="S103" s="42" t="s">
+      <c r="S103" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="T103" s="42" t="s">
+      <c r="T103" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="U103" s="43">
+      <c r="U103" s="42">
         <v>42449</v>
       </c>
-      <c r="V103" s="44">
-        <v>0</v>
-      </c>
-      <c r="W103" s="42" t="s">
+      <c r="V103" s="43">
+        <v>0</v>
+      </c>
+      <c r="W103" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="X103" s="42" t="s">
+      <c r="X103" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="Y103" s="45" t="s">
+      <c r="Y103" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="Z103" s="44">
+      <c r="Z103" s="43">
         <v>999</v>
       </c>
-      <c r="AA103" s="44">
+      <c r="AA103" s="43">
         <v>60</v>
       </c>
-      <c r="AB103" s="43"/>
-      <c r="AC103" s="43"/>
-      <c r="AD103" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE103" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF103" s="44">
+      <c r="AB103" s="42"/>
+      <c r="AC103" s="42"/>
+      <c r="AD103" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE103" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF103" s="43">
         <v>5</v>
       </c>
-      <c r="AG103" s="44">
+      <c r="AG103" s="43">
         <v>5</v>
       </c>
-      <c r="AH103" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI103" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ103" s="42" t="s">
+      <c r="AH103" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI103" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ103" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="AK103" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL103" s="42" t="s">
+      <c r="AK103" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL103" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM103" s="42" t="s">
+      <c r="AM103" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN103" s="42" t="s">
+      <c r="AN103" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="AO103" s="47"/>
-      <c r="AP103" s="47"/>
+      <c r="AO103" s="46"/>
+      <c r="AP103" s="46"/>
     </row>
     <row r="104" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A104" s="42" t="s">
+      <c r="A104" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B104" s="42"/>
-      <c r="C104" s="42"/>
-      <c r="D104" s="42"/>
-      <c r="E104" s="42"/>
-      <c r="F104" s="43"/>
-      <c r="G104" s="44"/>
-      <c r="H104" s="44"/>
-      <c r="I104" s="44"/>
-      <c r="J104" s="43"/>
-      <c r="K104" s="44"/>
-      <c r="L104" s="45"/>
-      <c r="M104" s="43">
+      <c r="B104" s="41"/>
+      <c r="C104" s="41"/>
+      <c r="D104" s="41"/>
+      <c r="E104" s="41"/>
+      <c r="F104" s="42"/>
+      <c r="G104" s="43"/>
+      <c r="H104" s="43"/>
+      <c r="I104" s="43"/>
+      <c r="J104" s="42"/>
+      <c r="K104" s="43"/>
+      <c r="L104" s="44"/>
+      <c r="M104" s="42">
         <v>42461</v>
       </c>
-      <c r="N104" s="43">
+      <c r="N104" s="42">
         <v>42466</v>
       </c>
-      <c r="O104" s="44">
+      <c r="O104" s="43">
         <v>4</v>
       </c>
-      <c r="P104" s="46" t="s">
+      <c r="P104" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="Q104" s="42" t="s">
+      <c r="Q104" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="R104" s="44">
+      <c r="R104" s="43">
         <v>3</v>
       </c>
-      <c r="S104" s="42" t="s">
+      <c r="S104" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="T104" s="42" t="s">
+      <c r="T104" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="U104" s="43">
+      <c r="U104" s="42">
         <v>42466</v>
       </c>
-      <c r="V104" s="44">
-        <v>0</v>
-      </c>
-      <c r="W104" s="42" t="s">
+      <c r="V104" s="43">
+        <v>0</v>
+      </c>
+      <c r="W104" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="X104" s="42" t="s">
+      <c r="X104" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="Y104" s="45" t="s">
+      <c r="Y104" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="Z104" s="44"/>
-      <c r="AA104" s="44"/>
-      <c r="AB104" s="43">
+      <c r="Z104" s="43"/>
+      <c r="AA104" s="43"/>
+      <c r="AB104" s="42">
         <v>42088</v>
       </c>
-      <c r="AC104" s="43">
+      <c r="AC104" s="42">
         <v>42369</v>
       </c>
-      <c r="AD104" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE104" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF104" s="44">
+      <c r="AD104" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE104" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF104" s="43">
         <v>4</v>
       </c>
-      <c r="AG104" s="44">
+      <c r="AG104" s="43">
         <v>4</v>
       </c>
-      <c r="AH104" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI104" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ104" s="42" t="s">
+      <c r="AH104" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI104" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ104" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="AK104" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL104" s="42" t="s">
+      <c r="AK104" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL104" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM104" s="42" t="s">
+      <c r="AM104" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN104" s="42" t="s">
+      <c r="AN104" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="AO104" s="47"/>
-      <c r="AP104" s="47"/>
+      <c r="AO104" s="46"/>
+      <c r="AP104" s="46"/>
     </row>
     <row r="105" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A105" s="42" t="s">
+      <c r="A105" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B105" s="42"/>
-      <c r="C105" s="42"/>
-      <c r="D105" s="42"/>
-      <c r="E105" s="42"/>
-      <c r="F105" s="43"/>
-      <c r="G105" s="44"/>
-      <c r="H105" s="44"/>
-      <c r="I105" s="44"/>
-      <c r="J105" s="43"/>
-      <c r="K105" s="44"/>
-      <c r="L105" s="45"/>
-      <c r="M105" s="43">
+      <c r="B105" s="41"/>
+      <c r="C105" s="41"/>
+      <c r="D105" s="41"/>
+      <c r="E105" s="41"/>
+      <c r="F105" s="42"/>
+      <c r="G105" s="43"/>
+      <c r="H105" s="43"/>
+      <c r="I105" s="43"/>
+      <c r="J105" s="42"/>
+      <c r="K105" s="43"/>
+      <c r="L105" s="44"/>
+      <c r="M105" s="42">
         <v>42491</v>
       </c>
-      <c r="N105" s="43">
+      <c r="N105" s="42">
         <v>42495</v>
       </c>
-      <c r="O105" s="44">
+      <c r="O105" s="43">
         <v>5</v>
       </c>
-      <c r="P105" s="46" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q105" s="42" t="s">
+      <c r="P105" s="45" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q105" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="R105" s="44">
+      <c r="R105" s="43">
         <v>4</v>
       </c>
-      <c r="S105" s="42" t="s">
+      <c r="S105" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="T105" s="42" t="s">
+      <c r="T105" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="U105" s="43">
+      <c r="U105" s="42">
         <v>42500</v>
       </c>
-      <c r="V105" s="44">
-        <v>0</v>
-      </c>
-      <c r="W105" s="42" t="s">
+      <c r="V105" s="43">
+        <v>0</v>
+      </c>
+      <c r="W105" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="X105" s="42" t="s">
+      <c r="X105" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="Y105" s="45" t="s">
+      <c r="Y105" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="Z105" s="44"/>
-      <c r="AA105" s="44"/>
-      <c r="AB105" s="43"/>
-      <c r="AC105" s="43"/>
-      <c r="AD105" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE105" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF105" s="44">
+      <c r="Z105" s="43"/>
+      <c r="AA105" s="43"/>
+      <c r="AB105" s="42"/>
+      <c r="AC105" s="42"/>
+      <c r="AD105" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE105" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF105" s="43">
         <v>5</v>
       </c>
-      <c r="AG105" s="44">
+      <c r="AG105" s="43">
         <v>5</v>
       </c>
-      <c r="AH105" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI105" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ105" s="42" t="s">
+      <c r="AH105" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI105" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ105" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="AK105" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL105" s="42" t="s">
+      <c r="AK105" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL105" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM105" s="42" t="s">
+      <c r="AM105" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN105" s="42" t="s">
+      <c r="AN105" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="AO105" s="47"/>
-      <c r="AP105" s="47"/>
+      <c r="AO105" s="46"/>
+      <c r="AP105" s="46"/>
     </row>
     <row r="106" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A106" s="42" t="s">
+      <c r="A106" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B106" s="42"/>
-      <c r="C106" s="42"/>
-      <c r="D106" s="42"/>
-      <c r="E106" s="42"/>
-      <c r="F106" s="43"/>
-      <c r="G106" s="44"/>
-      <c r="H106" s="44"/>
-      <c r="I106" s="44"/>
-      <c r="J106" s="43"/>
-      <c r="K106" s="44"/>
-      <c r="L106" s="45"/>
-      <c r="M106" s="43">
+      <c r="B106" s="41"/>
+      <c r="C106" s="41"/>
+      <c r="D106" s="41"/>
+      <c r="E106" s="41"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="43"/>
+      <c r="H106" s="43"/>
+      <c r="I106" s="43"/>
+      <c r="J106" s="42"/>
+      <c r="K106" s="43"/>
+      <c r="L106" s="44"/>
+      <c r="M106" s="42">
         <v>42496</v>
       </c>
-      <c r="N106" s="43">
+      <c r="N106" s="42">
         <v>42500</v>
       </c>
-      <c r="O106" s="44">
+      <c r="O106" s="43">
         <v>4</v>
       </c>
-      <c r="P106" s="46" t="s">
+      <c r="P106" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="Q106" s="42" t="s">
+      <c r="Q106" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="R106" s="44">
+      <c r="R106" s="43">
         <v>3</v>
       </c>
-      <c r="S106" s="42" t="s">
+      <c r="S106" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="T106" s="42" t="s">
+      <c r="T106" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="U106" s="43">
+      <c r="U106" s="42">
         <v>42500</v>
       </c>
-      <c r="V106" s="44">
-        <v>0</v>
-      </c>
-      <c r="W106" s="42" t="s">
+      <c r="V106" s="43">
+        <v>0</v>
+      </c>
+      <c r="W106" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="X106" s="42" t="s">
+      <c r="X106" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="Y106" s="45" t="s">
+      <c r="Y106" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="Z106" s="44"/>
-      <c r="AA106" s="44"/>
-      <c r="AB106" s="43"/>
-      <c r="AC106" s="43"/>
-      <c r="AD106" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE106" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF106" s="44">
+      <c r="Z106" s="43"/>
+      <c r="AA106" s="43"/>
+      <c r="AB106" s="42"/>
+      <c r="AC106" s="42"/>
+      <c r="AD106" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE106" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF106" s="43">
         <v>4</v>
       </c>
-      <c r="AG106" s="44">
+      <c r="AG106" s="43">
         <v>4</v>
       </c>
-      <c r="AH106" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI106" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ106" s="42" t="s">
+      <c r="AH106" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI106" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ106" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="AK106" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL106" s="42" t="s">
+      <c r="AK106" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL106" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM106" s="42" t="s">
+      <c r="AM106" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN106" s="42" t="s">
+      <c r="AN106" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="AO106" s="47"/>
-      <c r="AP106" s="47"/>
-    </row>
-    <row r="107" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A107" s="42" t="s">
+      <c r="AO106" s="46"/>
+      <c r="AP106" s="46"/>
+    </row>
+    <row r="107" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B107" s="42"/>
-      <c r="C107" s="42"/>
-      <c r="D107" s="42"/>
-      <c r="E107" s="42"/>
-      <c r="F107" s="43"/>
-      <c r="G107" s="44"/>
-      <c r="H107" s="44"/>
-      <c r="I107" s="44"/>
-      <c r="J107" s="43"/>
-      <c r="K107" s="44"/>
-      <c r="L107" s="45"/>
-      <c r="M107" s="43">
+      <c r="B107" s="41"/>
+      <c r="C107" s="41"/>
+      <c r="D107" s="41"/>
+      <c r="E107" s="41"/>
+      <c r="F107" s="42"/>
+      <c r="G107" s="43"/>
+      <c r="H107" s="43"/>
+      <c r="I107" s="43"/>
+      <c r="J107" s="42"/>
+      <c r="K107" s="43"/>
+      <c r="L107" s="44"/>
+      <c r="M107" s="42">
         <v>42502</v>
       </c>
-      <c r="N107" s="43">
+      <c r="N107" s="42">
         <v>42515</v>
       </c>
-      <c r="O107" s="44">
+      <c r="O107" s="43">
         <v>14</v>
       </c>
-      <c r="P107" s="46" t="s">
+      <c r="P107" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="Q107" s="42" t="s">
+      <c r="Q107" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="R107" s="44">
+      <c r="R107" s="43">
         <v>6</v>
       </c>
-      <c r="S107" s="42" t="s">
+      <c r="S107" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="T107" s="42" t="s">
+      <c r="T107" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="U107" s="43">
+      <c r="U107" s="42">
         <v>42530</v>
       </c>
-      <c r="V107" s="44">
+      <c r="V107" s="43">
         <v>2</v>
       </c>
-      <c r="W107" s="42" t="s">
+      <c r="W107" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="X107" s="42" t="s">
+      <c r="X107" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="Y107" s="45" t="s">
+      <c r="Y107" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="Z107" s="44"/>
-      <c r="AA107" s="44"/>
-      <c r="AB107" s="43"/>
-      <c r="AC107" s="43"/>
-      <c r="AD107" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE107" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF107" s="44">
+      <c r="Z107" s="43"/>
+      <c r="AA107" s="43"/>
+      <c r="AB107" s="42"/>
+      <c r="AC107" s="42"/>
+      <c r="AD107" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE107" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF107" s="43">
         <v>7</v>
       </c>
-      <c r="AG107" s="44">
+      <c r="AG107" s="43">
         <v>7</v>
       </c>
-      <c r="AH107" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI107" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ107" s="42" t="s">
+      <c r="AH107" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI107" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ107" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="AK107" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL107" s="42" t="s">
+      <c r="AK107" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL107" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM107" s="42" t="s">
+      <c r="AM107" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN107" s="42" t="s">
+      <c r="AN107" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="AO107" s="47"/>
-      <c r="AP107" s="47"/>
+      <c r="AO107" s="46"/>
+      <c r="AP107" s="46"/>
     </row>
     <row r="108" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A108" s="42" t="s">
+      <c r="A108" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B108" s="42"/>
-      <c r="C108" s="42"/>
-      <c r="D108" s="42"/>
-      <c r="E108" s="42"/>
-      <c r="F108" s="43"/>
-      <c r="G108" s="44"/>
-      <c r="H108" s="44"/>
-      <c r="I108" s="44"/>
-      <c r="J108" s="43"/>
-      <c r="K108" s="44"/>
-      <c r="L108" s="45"/>
-      <c r="M108" s="43">
+      <c r="B108" s="41"/>
+      <c r="C108" s="41"/>
+      <c r="D108" s="41"/>
+      <c r="E108" s="41"/>
+      <c r="F108" s="42"/>
+      <c r="G108" s="43"/>
+      <c r="H108" s="43"/>
+      <c r="I108" s="43"/>
+      <c r="J108" s="42"/>
+      <c r="K108" s="43"/>
+      <c r="L108" s="44"/>
+      <c r="M108" s="42">
         <v>42516</v>
       </c>
-      <c r="N108" s="43">
+      <c r="N108" s="42">
         <v>42530</v>
       </c>
-      <c r="O108" s="44">
+      <c r="O108" s="43">
         <v>5</v>
       </c>
-      <c r="P108" s="46" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q108" s="42" t="s">
+      <c r="P108" s="45" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q108" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="R108" s="44">
+      <c r="R108" s="43">
         <v>4</v>
       </c>
-      <c r="S108" s="42" t="s">
+      <c r="S108" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="T108" s="42" t="s">
+      <c r="T108" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="U108" s="43">
+      <c r="U108" s="42">
         <v>42530</v>
       </c>
-      <c r="V108" s="44">
+      <c r="V108" s="43">
         <v>2</v>
       </c>
-      <c r="W108" s="42" t="s">
+      <c r="W108" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="X108" s="42" t="s">
+      <c r="X108" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="Y108" s="45" t="s">
+      <c r="Y108" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="Z108" s="44"/>
-      <c r="AA108" s="44"/>
-      <c r="AB108" s="43"/>
-      <c r="AC108" s="43"/>
-      <c r="AD108" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE108" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF108" s="44">
+      <c r="Z108" s="43"/>
+      <c r="AA108" s="43"/>
+      <c r="AB108" s="42"/>
+      <c r="AC108" s="42"/>
+      <c r="AD108" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE108" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF108" s="43">
         <v>5</v>
       </c>
-      <c r="AG108" s="44">
+      <c r="AG108" s="43">
         <v>5</v>
       </c>
-      <c r="AH108" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI108" s="44">
-        <v>0</v>
-      </c>
-      <c r="AJ108" s="42" t="s">
+      <c r="AH108" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI108" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ108" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="AK108" s="47">
-        <v>0</v>
-      </c>
-      <c r="AL108" s="42" t="s">
+      <c r="AK108" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL108" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="AM108" s="42" t="s">
+      <c r="AM108" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AN108" s="42" t="s">
+      <c r="AN108" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="AO108" s="47"/>
-      <c r="AP108" s="47"/>
+      <c r="AO108" s="46"/>
+      <c r="AP108" s="46"/>
+    </row>
+    <row r="109" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A109" s="41"/>
+      <c r="B109" s="41"/>
+      <c r="C109" s="41"/>
+      <c r="D109" s="41"/>
+      <c r="E109" s="41"/>
+      <c r="F109" s="42"/>
+      <c r="G109" s="43"/>
+      <c r="H109" s="43"/>
+      <c r="I109" s="43"/>
+      <c r="J109" s="42"/>
+      <c r="K109" s="43"/>
+      <c r="L109" s="44"/>
+      <c r="M109" s="42"/>
+      <c r="N109" s="42"/>
+      <c r="O109" s="43"/>
+      <c r="P109" s="45"/>
+      <c r="Q109" s="41"/>
+      <c r="R109" s="43"/>
+      <c r="S109" s="41"/>
+      <c r="T109" s="41"/>
+      <c r="U109" s="42"/>
+      <c r="V109" s="43"/>
+      <c r="W109" s="41"/>
+      <c r="X109" s="41"/>
+      <c r="Y109" s="44"/>
+      <c r="Z109" s="43"/>
+      <c r="AA109" s="43"/>
+      <c r="AB109" s="42"/>
+      <c r="AC109" s="42"/>
+      <c r="AD109" s="43"/>
+      <c r="AE109" s="43"/>
+      <c r="AF109" s="43"/>
+      <c r="AG109" s="43"/>
+      <c r="AH109" s="43"/>
+      <c r="AI109" s="43"/>
+      <c r="AJ109" s="41"/>
+      <c r="AK109" s="46"/>
+      <c r="AL109" s="41"/>
+      <c r="AM109" s="41"/>
+      <c r="AN109" s="41"/>
+      <c r="AO109" s="46"/>
+      <c r="AP109" s="46"/>
+    </row>
+    <row r="110" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+      <c r="A110" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B110" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C110" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D110" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E110" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F110" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="G110" s="43">
+        <v>1</v>
+      </c>
+      <c r="H110" s="43">
+        <v>0</v>
+      </c>
+      <c r="I110" s="43">
+        <v>0</v>
+      </c>
+      <c r="J110" s="42">
+        <v>42396</v>
+      </c>
+      <c r="K110" s="43">
+        <v>13</v>
+      </c>
+      <c r="L110" s="44" t="s">
+        <v>308</v>
+      </c>
+      <c r="M110" s="42">
+        <v>42396</v>
+      </c>
+      <c r="N110" s="42">
+        <v>42396</v>
+      </c>
+      <c r="O110" s="43">
+        <v>13</v>
+      </c>
+      <c r="P110" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q110" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="R110" s="43">
+        <v>5</v>
+      </c>
+      <c r="S110" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="T110" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="U110" s="42">
+        <v>42402</v>
+      </c>
+      <c r="V110" s="43">
+        <v>3</v>
+      </c>
+      <c r="W110" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="X110" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y110" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z110" s="43">
+        <v>999</v>
+      </c>
+      <c r="AA110" s="43">
+        <v>1</v>
+      </c>
+      <c r="AB110" s="42"/>
+      <c r="AC110" s="42"/>
+      <c r="AD110" s="43">
+        <v>0</v>
+      </c>
+      <c r="AE110" s="43">
+        <v>0</v>
+      </c>
+      <c r="AF110" s="43">
+        <v>6</v>
+      </c>
+      <c r="AG110" s="43">
+        <v>7</v>
+      </c>
+      <c r="AH110" s="43">
+        <v>0</v>
+      </c>
+      <c r="AI110" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ110" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK110" s="46">
+        <v>-11</v>
+      </c>
+      <c r="AL110" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM110" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN110" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO110" s="46">
+        <v>-471.92</v>
+      </c>
+      <c r="AP110" s="46">
+        <v>1809.08</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added column for scripting SpecialOffer test
</commit_message>
<xml_diff>
--- a/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
+++ b/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\github\OltSchema\BaseData\HotelExport\SpecialOffers\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" r:id="rId1"/>
     <sheet name="Result" sheetId="6" r:id="rId2"/>
-    <sheet name="Tabelle1" sheetId="7" r:id="rId3"/>
-    <sheet name="PreisProTag" sheetId="4" r:id="rId4"/>
-    <sheet name="ToDo" sheetId="5" r:id="rId5"/>
-    <sheet name="ResultOld" sheetId="2" r:id="rId6"/>
+    <sheet name="PreisProTag" sheetId="4" r:id="rId3"/>
+    <sheet name="ToDo" sheetId="5" r:id="rId4"/>
+    <sheet name="ResultOld" sheetId="2" r:id="rId5"/>
+    <sheet name="BasisFürTestSkript" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3523" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3521" uniqueCount="315">
   <si>
     <t>ItemType</t>
   </si>
@@ -1005,13 +1010,23 @@
 (27.01.16-02.02.16) Average / 149.71 - 11 = 138.71 
 (03.02.16-08.02.16) Average / 205.50 - 11 = 194.50 </t>
   </si>
+  <si>
+    <t>BookDate</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>BookStart</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mmm\ d&quot;, &quot;yy"/>
+    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -1624,7 +1639,7 @@
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1765,6 +1780,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="57" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="10" xfId="57" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
@@ -2895,7 +2914,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -19050,8 +19069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB30" sqref="A30:XFD30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30264,63 +30283,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="12" max="12" width="37.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="29">
-        <v>1</v>
-      </c>
-      <c r="H3" s="29">
-        <v>0</v>
-      </c>
-      <c r="I3" s="29">
-        <v>0</v>
-      </c>
-      <c r="J3" s="31">
-        <v>42430</v>
-      </c>
-      <c r="K3" s="29">
-        <v>30</v>
-      </c>
-      <c r="L3" s="30" t="s">
-        <v>188</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K368"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -33298,7 +33260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -33354,7 +33316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ95"/>
   <sheetViews>
@@ -43576,4 +43538,2885 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L110"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="K108" sqref="K108"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="49"/>
+    <col min="5" max="5" width="14.28515625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="49"/>
+    <col min="7" max="7" width="56.5703125" customWidth="1"/>
+    <col min="12" max="12" width="37.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(2,</v>
+      </c>
+      <c r="B2" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C2" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>3,</v>
+      </c>
+      <c r="E2" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G2" t="str">
+        <f ca="1">CONCATENATE(A2,B2,C2,D2,E2)</f>
+        <v>(2,'TUIXYA225410','2016-01-01',3,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(3,</v>
+      </c>
+      <c r="B3" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C3" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D3" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>4,</v>
+      </c>
+      <c r="E3" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="F3" s="50"/>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G66" ca="1" si="0">CONCATENATE(A3,B3,C3,D3,E3)</f>
+        <v>(3,'TUIXYA225410','2016-01-01',4,'2015-05-19'),</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="30"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(4,</v>
+      </c>
+      <c r="B4" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C4" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E4" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(4,'TUIXYA225410','2016-01-01',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(5,</v>
+      </c>
+      <c r="B5" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C5" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D5" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>6,</v>
+      </c>
+      <c r="E5" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(5,'TUIXYA225410','2016-01-01',6,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(6,</v>
+      </c>
+      <c r="B6" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C6" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E6" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(6,'TUIXYA225410','2016-01-01',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(7,</v>
+      </c>
+      <c r="B7" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C7" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>8,</v>
+      </c>
+      <c r="E7" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(7,'TUIXYA225410','2016-01-01',8,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(8,</v>
+      </c>
+      <c r="B8" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C8" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D8" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>9,</v>
+      </c>
+      <c r="E8" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(8,'TUIXYA225410','2016-01-01',9,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(9,</v>
+      </c>
+      <c r="B9" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C9" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>10,</v>
+      </c>
+      <c r="E9" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(9,'TUIXYA225410','2016-01-01',10,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(10,</v>
+      </c>
+      <c r="B10" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C10" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D10" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>11,</v>
+      </c>
+      <c r="E10" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(10,'TUIXYA225410','2016-01-01',11,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(11,</v>
+      </c>
+      <c r="B11" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C11" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D11" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>12,</v>
+      </c>
+      <c r="E11" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(11,'TUIXYA225410','2016-01-01',12,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(12,</v>
+      </c>
+      <c r="B12" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C12" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E12" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(12,'TUIXYA225410','2016-01-01',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(13,</v>
+      </c>
+      <c r="B13" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C13" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D13" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>14,</v>
+      </c>
+      <c r="E13" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(13,'TUIXYA225410','2016-01-01',14,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(14,</v>
+      </c>
+      <c r="B14" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C14" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D14" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>15,</v>
+      </c>
+      <c r="E14" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(14,'TUIXYA225410','2016-01-01',15,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(15,</v>
+      </c>
+      <c r="B15" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C15" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D15" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>16,</v>
+      </c>
+      <c r="E15" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(15,'TUIXYA225410','2016-01-01',16,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(16,</v>
+      </c>
+      <c r="B16" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C16" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D16" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>17,</v>
+      </c>
+      <c r="E16" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(16,'TUIXYA225410','2016-01-01',17,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(17,</v>
+      </c>
+      <c r="B17" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C17" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D17" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>18,</v>
+      </c>
+      <c r="E17" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(17,'TUIXYA225410','2016-01-01',18,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C18" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E18" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(19,</v>
+      </c>
+      <c r="B19" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C19" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D19" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>19,</v>
+      </c>
+      <c r="E19" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(19,'TUIXYA225410','2016-01-01',19,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C20" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E20" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(21,</v>
+      </c>
+      <c r="B21" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C21" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>20,</v>
+      </c>
+      <c r="E21" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(21,'TUIXYA225410','2016-01-01',20,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(22,</v>
+      </c>
+      <c r="B22" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C22" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D22" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>21,</v>
+      </c>
+      <c r="E22" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(22,'TUIXYA225410','2016-01-01',21,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(23,</v>
+      </c>
+      <c r="B23" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C23" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D23" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>22,</v>
+      </c>
+      <c r="E23" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(23,'TUIXYA225410','2016-01-01',22,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(24,</v>
+      </c>
+      <c r="B24" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C24" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D24" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>23,</v>
+      </c>
+      <c r="E24" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(24,'TUIXYA225410','2016-01-01',23,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B25" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C25" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D25" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E25" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(26,</v>
+      </c>
+      <c r="B26" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C26" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-23',</v>
+      </c>
+      <c r="D26" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E26" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(26,'TUIXYA225410','2016-01-23',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(27,</v>
+      </c>
+      <c r="B27" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C27" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-24',</v>
+      </c>
+      <c r="D27" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E27" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(27,'TUIXYA225410','2016-01-24',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(28,</v>
+      </c>
+      <c r="B28" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C28" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-25',</v>
+      </c>
+      <c r="D28" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E28" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(28,'TUIXYA225410','2016-01-25',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(29,</v>
+      </c>
+      <c r="B29" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C29" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-26',</v>
+      </c>
+      <c r="D29" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E29" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(29,'TUIXYA225410','2016-01-26',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(30,</v>
+      </c>
+      <c r="B30" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C30" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-27',</v>
+      </c>
+      <c r="D30" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E30" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(30,'TUIXYA225410','2016-01-27',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B31" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C31" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D31" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E31" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(32,</v>
+      </c>
+      <c r="B32" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C32" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-28',</v>
+      </c>
+      <c r="D32" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E32" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(32,'TUIXYA225410','2016-01-28',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(33,</v>
+      </c>
+      <c r="B33" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C33" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-29',</v>
+      </c>
+      <c r="D33" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E33" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(33,'TUIXYA225410','2016-01-29',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(34,</v>
+      </c>
+      <c r="B34" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C34" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-30',</v>
+      </c>
+      <c r="D34" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E34" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(34,'TUIXYA225410','2016-01-30',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(35,</v>
+      </c>
+      <c r="B35" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C35" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-31',</v>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E35" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(35,'TUIXYA225410','2016-01-31',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(36,</v>
+      </c>
+      <c r="B36" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C36" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-01',</v>
+      </c>
+      <c r="D36" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E36" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(36,'TUIXYA225410','2016-02-01',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(37,</v>
+      </c>
+      <c r="B37" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C37" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-02',</v>
+      </c>
+      <c r="D37" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E37" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(37,'TUIXYA225410','2016-02-02',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B38" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C38" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D38" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E38" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(39,</v>
+      </c>
+      <c r="B39" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C39" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-03',</v>
+      </c>
+      <c r="D39" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E39" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(39,'TUIXYA225410','2016-02-03',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(40,</v>
+      </c>
+      <c r="B40" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C40" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-04',</v>
+      </c>
+      <c r="D40" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E40" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(40,'TUIXYA225410','2016-02-04',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(41,</v>
+      </c>
+      <c r="B41" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C41" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-09',</v>
+      </c>
+      <c r="D41" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E41" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(41,'TUIXYA225410','2016-02-09',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(42,</v>
+      </c>
+      <c r="B42" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C42" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-10',</v>
+      </c>
+      <c r="D42" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E42" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(42,'TUIXYA225410','2016-02-10',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(43,</v>
+      </c>
+      <c r="B43" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C43" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-15',</v>
+      </c>
+      <c r="D43" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E43" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(43,'TUIXYA225410','2016-02-15',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(44,</v>
+      </c>
+      <c r="B44" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C44" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-16',</v>
+      </c>
+      <c r="D44" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>7,</v>
+      </c>
+      <c r="E44" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(44,'TUIXYA225410','2016-02-16',7,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B45" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C45" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D45" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E45" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(46,</v>
+      </c>
+      <c r="B46" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C46" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-18',</v>
+      </c>
+      <c r="D46" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E46" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(46,'TUIXYA225410','2016-02-18',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(47,</v>
+      </c>
+      <c r="B47" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C47" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-19',</v>
+      </c>
+      <c r="D47" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E47" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(47,'TUIXYA225410','2016-02-19',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(48,</v>
+      </c>
+      <c r="B48" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C48" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-23',</v>
+      </c>
+      <c r="D48" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E48" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(48,'TUIXYA225410','2016-02-23',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(49,</v>
+      </c>
+      <c r="B49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C49" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-24',</v>
+      </c>
+      <c r="D49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E49" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(49,'TUIXYA225410','2016-02-24',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B50" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C50" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D50" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E50" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(51,</v>
+      </c>
+      <c r="B51" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C51" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-28',</v>
+      </c>
+      <c r="D51" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E51" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(51,'TUIXYA225410','2016-02-28',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(52,</v>
+      </c>
+      <c r="B52" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C52" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-02-29',</v>
+      </c>
+      <c r="D52" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E52" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(52,'TUIXYA225410','2016-02-29',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(53,</v>
+      </c>
+      <c r="B53" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C53" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-03-01',</v>
+      </c>
+      <c r="D53" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E53" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(53,'TUIXYA225410','2016-03-01',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(54,</v>
+      </c>
+      <c r="B54" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C54" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-03-02',</v>
+      </c>
+      <c r="D54" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E54" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(54,'TUIXYA225410','2016-03-02',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(55,</v>
+      </c>
+      <c r="B55" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C55" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-03-03',</v>
+      </c>
+      <c r="D55" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E55" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(55,'TUIXYA225410','2016-03-03',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B56" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C56" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D56" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E56" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(57,</v>
+      </c>
+      <c r="B57" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C57" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-03-07',</v>
+      </c>
+      <c r="D57" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E57" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(57,'TUIXYA225410','2016-03-07',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(58,</v>
+      </c>
+      <c r="B58" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C58" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-03-14',</v>
+      </c>
+      <c r="D58" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E58" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-08-01'),</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(58,'TUIXYA225410','2016-03-14',5,'2015-08-01'),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(59,</v>
+      </c>
+      <c r="B59" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C59" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-03-22',</v>
+      </c>
+      <c r="D59" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E59" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2016-02-10'),</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(59,'TUIXYA225410','2016-03-22',5,'2016-02-10'),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B60" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C60" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D60" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E60" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(61,</v>
+      </c>
+      <c r="B61" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C61" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-04-01',</v>
+      </c>
+      <c r="D61" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E61" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-08-01'),</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(61,'TUIXYA225410','2016-04-01',5,'2015-08-01'),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(62,</v>
+      </c>
+      <c r="B62" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C62" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-04-08',</v>
+      </c>
+      <c r="D62" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E62" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2016-02-02'),</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(62,'TUIXYA225410','2016-04-08',5,'2016-02-02'),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(63,</v>
+      </c>
+      <c r="B63" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C63" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-04-01',</v>
+      </c>
+      <c r="D63" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>15,</v>
+      </c>
+      <c r="E63" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2016-03-10'),</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(63,'TUIXYA225410','2016-04-01',15,'2016-03-10'),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B64" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C64" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D64" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E64" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(65,</v>
+      </c>
+      <c r="B65" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C65" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-01',</v>
+      </c>
+      <c r="D65" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E65" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(65,'TUIXYA225410','2016-05-01',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(66,</v>
+      </c>
+      <c r="B66" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C66" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-02',</v>
+      </c>
+      <c r="D66" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E66" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(66,'TUIXYA225410','2016-05-02',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(67,</v>
+      </c>
+      <c r="B67" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C67" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-03',</v>
+      </c>
+      <c r="D67" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E67" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" ref="G67:G110" ca="1" si="1">CONCATENATE(A67,B67,C67,D67,E67)</f>
+        <v>(67,'TUIXYA225410','2016-05-03',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(68,</v>
+      </c>
+      <c r="B68" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C68" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-04',</v>
+      </c>
+      <c r="D68" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E68" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(68,'TUIXYA225410','2016-05-04',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(69,</v>
+      </c>
+      <c r="B69" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C69" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-05',</v>
+      </c>
+      <c r="D69" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E69" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(69,'TUIXYA225410','2016-05-05',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(70,</v>
+      </c>
+      <c r="B70" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C70" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-06',</v>
+      </c>
+      <c r="D70" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E70" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(70,'TUIXYA225410','2016-05-06',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(71,</v>
+      </c>
+      <c r="B71" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C71" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-07',</v>
+      </c>
+      <c r="D71" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E71" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(71,'TUIXYA225410','2016-05-07',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(72,</v>
+      </c>
+      <c r="B72" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C72" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-08',</v>
+      </c>
+      <c r="D72" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>5,</v>
+      </c>
+      <c r="E72" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(72,'TUIXYA225410','2016-05-08',5,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B73" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C73" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D73" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E73" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(74,</v>
+      </c>
+      <c r="B74" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C74" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-13',</v>
+      </c>
+      <c r="D74" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E74" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(74,'TUIXYA225410','2016-05-13',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(75,</v>
+      </c>
+      <c r="B75" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C75" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-14',</v>
+      </c>
+      <c r="D75" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E75" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(75,'TUIXYA225410','2016-05-14',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(76,</v>
+      </c>
+      <c r="B76" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C76" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-18',</v>
+      </c>
+      <c r="D76" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E76" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(76,'TUIXYA225410','2016-05-18',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B77" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C77" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D77" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E77" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(78,</v>
+      </c>
+      <c r="B78" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C78" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-19',</v>
+      </c>
+      <c r="D78" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E78" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(78,'TUIXYA225410','2016-05-19',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B79" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C79" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D79" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E79" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(80,</v>
+      </c>
+      <c r="B80" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C80" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-20',</v>
+      </c>
+      <c r="D80" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E80" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(80,'TUIXYA225410','2016-05-20',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B81" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C81" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D81" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E81" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(82,</v>
+      </c>
+      <c r="B82" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C82" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-21',</v>
+      </c>
+      <c r="D82" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E82" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(82,'TUIXYA225410','2016-05-21',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B83" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C83" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D83" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E83" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(84,</v>
+      </c>
+      <c r="B84" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C84" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-22',</v>
+      </c>
+      <c r="D84" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E84" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(84,'TUIXYA225410','2016-05-22',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B85" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C85" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D85" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E85" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(86,</v>
+      </c>
+      <c r="B86" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C86" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-23',</v>
+      </c>
+      <c r="D86" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E86" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(86,'TUIXYA225410','2016-05-23',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B87" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C87" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D87" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E87" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(88,</v>
+      </c>
+      <c r="B88" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C88" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-05-26',</v>
+      </c>
+      <c r="D88" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E88" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G88" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(88,'TUIXYA225410','2016-05-26',13,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B89" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C89" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D89" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E89" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(90,</v>
+      </c>
+      <c r="B90" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C90" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-07-03',</v>
+      </c>
+      <c r="D90" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>27,</v>
+      </c>
+      <c r="E90" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(90,'TUIXYA225410','2016-07-03',27,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B91" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C91" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D91" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E91" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B92" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C92" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D92" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E92" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(93,</v>
+      </c>
+      <c r="B93" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYZ50502',</v>
+      </c>
+      <c r="C93" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D93" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>3,</v>
+      </c>
+      <c r="E93" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G93" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(93,'TUIXYZ50502','2016-01-01',3,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(94,</v>
+      </c>
+      <c r="B94" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYZ50502',</v>
+      </c>
+      <c r="C94" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D94" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>3,</v>
+      </c>
+      <c r="E94" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G94" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(94,'TUIXYZ50502','2016-01-01',3,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(95,</v>
+      </c>
+      <c r="B95" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYZ50502',</v>
+      </c>
+      <c r="C95" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-01',</v>
+      </c>
+      <c r="D95" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>3,</v>
+      </c>
+      <c r="E95" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G95" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(95,'TUIXYZ50502','2016-01-01',3,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B96" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C96" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D96" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E96" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G96" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(97,</v>
+      </c>
+      <c r="B97" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C97" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-03-01',</v>
+      </c>
+      <c r="D97" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>30,</v>
+      </c>
+      <c r="E97" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G97" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(97,'TUIXYA225410','2016-03-01',30,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B98" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C98" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D98" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E98" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G98" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B99" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C99" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D99" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E99" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G99" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B100" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C100" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D100" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E100" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G100" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(101,</v>
+      </c>
+      <c r="B101" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C101" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-03-01',</v>
+      </c>
+      <c r="D101" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>91,</v>
+      </c>
+      <c r="E101" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(101,'TUIXYA225410','2016-03-01',91,'2015-05-19'),</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B102" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C102" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D102" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E102" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G102" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B103" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C103" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D103" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E103" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G103" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B104" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C104" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D104" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E104" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G104" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B105" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C105" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D105" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E105" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G105" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B106" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C106" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D106" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E106" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G106" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B107" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C107" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D107" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E107" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G107" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B108" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C108" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D108" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E108" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G108" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v/>
+      </c>
+      <c r="B109" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v/>
+      </c>
+      <c r="C109" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v/>
+      </c>
+      <c r="D109" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v/>
+      </c>
+      <c r="E109" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v/>
+      </c>
+      <c r="G109" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <v>(110,</v>
+      </c>
+      <c r="B110" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <v>'TUIXYA225410',</v>
+      </c>
+      <c r="C110" s="49" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <v>'2016-01-27',</v>
+      </c>
+      <c r="D110" t="str">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <v>13,</v>
+      </c>
+      <c r="E110" s="49" t="str">
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <v>'2015-05-19'),</v>
+      </c>
+      <c r="G110" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(110,'TUIXYA225410','2016-01-27',13,'2015-05-19'),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified the script generation for SpecialOffer tests
</commit_message>
<xml_diff>
--- a/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
+++ b/BaseData/HotelExport/SpecialOffers/SpecialPermutationen.xlsx
@@ -1026,7 +1026,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mmm\ d&quot;, &quot;yy"/>
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -1781,8 +1781,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="57" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="10" xfId="57" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="57" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -25788,7 +25788,7 @@
         <v>5295</v>
       </c>
     </row>
-    <row r="65" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:42" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
         <v>36</v>
       </c>
@@ -27372,7 +27372,7 @@
       <c r="AO79" s="26"/>
       <c r="AP79" s="26"/>
     </row>
-    <row r="80" spans="1:42" ht="360" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:42" ht="345" x14ac:dyDescent="0.25">
       <c r="A80" s="25" t="s">
         <v>36</v>
       </c>
@@ -43544,17 +43544,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="K108" sqref="K108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="49"/>
-    <col min="5" max="5" width="14.28515625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="49" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="49"/>
-    <col min="7" max="7" width="56.5703125" customWidth="1"/>
+    <col min="7" max="7" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -43576,55 +43578,55 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(2,</v>
+      <c r="A2">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>2</v>
       </c>
       <c r="B2" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C2" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>3,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D2">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>3</v>
       </c>
       <c r="E2" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G2" t="str">
-        <f ca="1">CONCATENATE(A2,B2,C2,D2,E2)</f>
+        <f ca="1">IF(LEN(B2)&gt;0,CONCATENATE("(",A2,",",B2,",",C2,",",D2,",",E2,"),"),"")</f>
         <v>(2,'TUIXYA225410','2016-01-01',3,'2015-05-19'),</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(3,</v>
+      <c r="A3">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>3</v>
       </c>
       <c r="B3" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C3" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D3" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>4,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D3">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>4</v>
       </c>
       <c r="E3" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="F3" s="50"/>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G66" ca="1" si="0">CONCATENATE(A3,B3,C3,D3,E3)</f>
+        <f t="shared" ref="G3:G66" ca="1" si="0">IF(LEN(B3)&gt;0,CONCATENATE("(",A3,",",B3,",",C3,",",D3,",",E3,"),"),"")</f>
         <v>(3,'TUIXYA225410','2016-01-01',4,'2015-05-19'),</v>
       </c>
       <c r="H3" s="29"/>
@@ -43634,25 +43636,25 @@
       <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(4,</v>
+      <c r="A4">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>4</v>
       </c>
       <c r="B4" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C4" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D4" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D4">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E4" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43660,25 +43662,25 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(5,</v>
+      <c r="A5">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>5</v>
       </c>
       <c r="B5" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C5" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D5" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>6,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D5">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>6</v>
       </c>
       <c r="E5" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43686,25 +43688,25 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(6,</v>
+      <c r="A6">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>6</v>
       </c>
       <c r="B6" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C6" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D6" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D6">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E6" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43712,25 +43714,25 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(7,</v>
+      <c r="A7">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>7</v>
       </c>
       <c r="B7" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C7" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D7" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>8,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D7">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>8</v>
       </c>
       <c r="E7" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43738,25 +43740,25 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(8,</v>
+      <c r="A8">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>8</v>
       </c>
       <c r="B8" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C8" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D8" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>9,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D8">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>9</v>
       </c>
       <c r="E8" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43764,25 +43766,25 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(9,</v>
+      <c r="A9">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>9</v>
       </c>
       <c r="B9" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C9" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D9" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>10,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D9">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>10</v>
       </c>
       <c r="E9" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43790,25 +43792,25 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(10,</v>
+      <c r="A10">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>10</v>
       </c>
       <c r="B10" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C10" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D10" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>11,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D10">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>11</v>
       </c>
       <c r="E10" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43816,25 +43818,25 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(11,</v>
+      <c r="A11">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>11</v>
       </c>
       <c r="B11" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C11" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D11" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>12,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D11">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>12</v>
       </c>
       <c r="E11" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43842,25 +43844,25 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(12,</v>
+      <c r="A12">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>12</v>
       </c>
       <c r="B12" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C12" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D12" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D12">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E12" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43868,25 +43870,25 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(13,</v>
+      <c r="A13">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>13</v>
       </c>
       <c r="B13" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C13" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D13" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>14,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D13">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>14</v>
       </c>
       <c r="E13" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43894,25 +43896,25 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(14,</v>
+      <c r="A14">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>14</v>
       </c>
       <c r="B14" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C14" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D14" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>15,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D14">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>15</v>
       </c>
       <c r="E14" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43920,25 +43922,25 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(15,</v>
+      <c r="A15">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>15</v>
       </c>
       <c r="B15" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C15" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D15" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>16,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D15">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>16</v>
       </c>
       <c r="E15" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43946,25 +43948,25 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(16,</v>
+      <c r="A16">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>16</v>
       </c>
       <c r="B16" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C16" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D16" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>17,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D16">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>17</v>
       </c>
       <c r="E16" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43972,25 +43974,25 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(17,</v>
+      <c r="A17">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>17</v>
       </c>
       <c r="B17" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C17" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D17" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>18,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D17">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>18</v>
       </c>
       <c r="E17" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43999,50 +44001,50 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B18" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C18" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D18" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E18" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G18" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(19,</v>
+      <c r="A19">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>19</v>
       </c>
       <c r="B19" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C19" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D19" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>19,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D19">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>19</v>
       </c>
       <c r="E19" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44051,50 +44053,50 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B20" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C20" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D20" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E20" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G20" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(21,</v>
+      <c r="A21">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>21</v>
       </c>
       <c r="B21" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C21" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D21" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>20,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D21">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>20</v>
       </c>
       <c r="E21" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44102,25 +44104,25 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(22,</v>
+      <c r="A22">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>22</v>
       </c>
       <c r="B22" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C22" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D22" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>21,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D22">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>21</v>
       </c>
       <c r="E22" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44128,25 +44130,25 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(23,</v>
+      <c r="A23">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>23</v>
       </c>
       <c r="B23" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C23" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D23" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>22,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D23">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>22</v>
       </c>
       <c r="E23" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44154,25 +44156,25 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(24,</v>
+      <c r="A24">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>24</v>
       </c>
       <c r="B24" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C24" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D24" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>23,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D24">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>23</v>
       </c>
       <c r="E24" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44181,50 +44183,50 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B25" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C25" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D25" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E25" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G25" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(26,</v>
+      <c r="A26">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>26</v>
       </c>
       <c r="B26" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C26" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-23',</v>
-      </c>
-      <c r="D26" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-23'</v>
+      </c>
+      <c r="D26">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E26" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44232,25 +44234,25 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(27,</v>
+      <c r="A27">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>27</v>
       </c>
       <c r="B27" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C27" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-24',</v>
-      </c>
-      <c r="D27" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-24'</v>
+      </c>
+      <c r="D27">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E27" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44258,25 +44260,25 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(28,</v>
+      <c r="A28">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>28</v>
       </c>
       <c r="B28" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C28" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-25',</v>
-      </c>
-      <c r="D28" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-25'</v>
+      </c>
+      <c r="D28">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E28" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44284,25 +44286,25 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(29,</v>
+      <c r="A29">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>29</v>
       </c>
       <c r="B29" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C29" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-26',</v>
-      </c>
-      <c r="D29" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-26'</v>
+      </c>
+      <c r="D29">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E29" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44310,25 +44312,25 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(30,</v>
+      <c r="A30">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>30</v>
       </c>
       <c r="B30" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C30" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-27',</v>
-      </c>
-      <c r="D30" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-27'</v>
+      </c>
+      <c r="D30">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E30" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44337,50 +44339,50 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B31" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C31" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D31" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E31" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G31" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(32,</v>
+      <c r="A32">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>32</v>
       </c>
       <c r="B32" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C32" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-28',</v>
-      </c>
-      <c r="D32" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-28'</v>
+      </c>
+      <c r="D32">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E32" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44388,25 +44390,25 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(33,</v>
+      <c r="A33">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>33</v>
       </c>
       <c r="B33" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C33" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-29',</v>
-      </c>
-      <c r="D33" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-29'</v>
+      </c>
+      <c r="D33">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E33" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44414,25 +44416,25 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(34,</v>
+      <c r="A34">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>34</v>
       </c>
       <c r="B34" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C34" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-30',</v>
-      </c>
-      <c r="D34" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-30'</v>
+      </c>
+      <c r="D34">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E34" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44440,25 +44442,25 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(35,</v>
+      <c r="A35">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>35</v>
       </c>
       <c r="B35" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C35" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-31',</v>
-      </c>
-      <c r="D35" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-31'</v>
+      </c>
+      <c r="D35">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E35" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44466,25 +44468,25 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(36,</v>
+      <c r="A36">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>36</v>
       </c>
       <c r="B36" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C36" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-01',</v>
-      </c>
-      <c r="D36" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-01'</v>
+      </c>
+      <c r="D36">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E36" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44492,25 +44494,25 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(37,</v>
+      <c r="A37">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>37</v>
       </c>
       <c r="B37" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C37" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-02',</v>
-      </c>
-      <c r="D37" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-02'</v>
+      </c>
+      <c r="D37">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E37" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44519,50 +44521,50 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B38" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C38" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D38" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E38" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G38" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(39,</v>
+      <c r="A39">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>39</v>
       </c>
       <c r="B39" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C39" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-03',</v>
-      </c>
-      <c r="D39" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-03'</v>
+      </c>
+      <c r="D39">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E39" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44570,25 +44572,25 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(40,</v>
+      <c r="A40">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>40</v>
       </c>
       <c r="B40" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C40" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-04',</v>
-      </c>
-      <c r="D40" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-04'</v>
+      </c>
+      <c r="D40">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E40" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44596,25 +44598,25 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(41,</v>
+      <c r="A41">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>41</v>
       </c>
       <c r="B41" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C41" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-09',</v>
-      </c>
-      <c r="D41" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-09'</v>
+      </c>
+      <c r="D41">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E41" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44622,25 +44624,25 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(42,</v>
+      <c r="A42">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>42</v>
       </c>
       <c r="B42" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C42" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-10',</v>
-      </c>
-      <c r="D42" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-10'</v>
+      </c>
+      <c r="D42">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E42" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44648,25 +44650,25 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(43,</v>
+      <c r="A43">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>43</v>
       </c>
       <c r="B43" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C43" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-15',</v>
-      </c>
-      <c r="D43" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-15'</v>
+      </c>
+      <c r="D43">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E43" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44674,25 +44676,25 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(44,</v>
+      <c r="A44">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>44</v>
       </c>
       <c r="B44" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C44" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-16',</v>
-      </c>
-      <c r="D44" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>7,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-16'</v>
+      </c>
+      <c r="D44">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>7</v>
       </c>
       <c r="E44" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44701,50 +44703,50 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B45" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C45" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D45" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E45" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G45" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(46,</v>
+      <c r="A46">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>46</v>
       </c>
       <c r="B46" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C46" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-18',</v>
-      </c>
-      <c r="D46" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-18'</v>
+      </c>
+      <c r="D46">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E46" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44752,25 +44754,25 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(47,</v>
+      <c r="A47">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>47</v>
       </c>
       <c r="B47" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C47" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-19',</v>
-      </c>
-      <c r="D47" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-19'</v>
+      </c>
+      <c r="D47">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E47" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44778,25 +44780,25 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(48,</v>
+      <c r="A48">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>48</v>
       </c>
       <c r="B48" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C48" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-23',</v>
-      </c>
-      <c r="D48" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-23'</v>
+      </c>
+      <c r="D48">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E48" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44804,25 +44806,25 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(49,</v>
+      <c r="A49">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>49</v>
       </c>
       <c r="B49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C49" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-24',</v>
-      </c>
-      <c r="D49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-24'</v>
+      </c>
+      <c r="D49">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E49" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44831,50 +44833,50 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B50" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C50" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D50" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E50" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G50" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(51,</v>
+      <c r="A51">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>51</v>
       </c>
       <c r="B51" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C51" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-28',</v>
-      </c>
-      <c r="D51" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-28'</v>
+      </c>
+      <c r="D51">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E51" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44882,25 +44884,25 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(52,</v>
+      <c r="A52">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>52</v>
       </c>
       <c r="B52" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C52" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-02-29',</v>
-      </c>
-      <c r="D52" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-02-29'</v>
+      </c>
+      <c r="D52">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E52" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44908,25 +44910,25 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(53,</v>
+      <c r="A53">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>53</v>
       </c>
       <c r="B53" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C53" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-03-01',</v>
-      </c>
-      <c r="D53" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-03-01'</v>
+      </c>
+      <c r="D53">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E53" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44934,25 +44936,25 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(54,</v>
+      <c r="A54">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>54</v>
       </c>
       <c r="B54" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C54" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-03-02',</v>
-      </c>
-      <c r="D54" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-03-02'</v>
+      </c>
+      <c r="D54">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E54" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44960,25 +44962,25 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(55,</v>
+      <c r="A55">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>55</v>
       </c>
       <c r="B55" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C55" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-03-03',</v>
-      </c>
-      <c r="D55" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-03-03'</v>
+      </c>
+      <c r="D55">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E55" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44987,50 +44989,50 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B56" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C56" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D56" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E56" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G56" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(57,</v>
+      <c r="A57">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>57</v>
       </c>
       <c r="B57" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C57" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-03-07',</v>
-      </c>
-      <c r="D57" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-03-07'</v>
+      </c>
+      <c r="D57">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E57" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45038,25 +45040,25 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(58,</v>
+      <c r="A58">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>58</v>
       </c>
       <c r="B58" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C58" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-03-14',</v>
-      </c>
-      <c r="D58" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-03-14'</v>
+      </c>
+      <c r="D58">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E58" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-08-01'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-08-01'</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45064,25 +45066,25 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(59,</v>
+      <c r="A59">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>59</v>
       </c>
       <c r="B59" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C59" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-03-22',</v>
-      </c>
-      <c r="D59" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-03-22'</v>
+      </c>
+      <c r="D59">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E59" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2016-02-10'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2016-02-10'</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45091,50 +45093,50 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B60" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C60" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D60" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E60" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G60" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(61,</v>
+      <c r="A61">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>61</v>
       </c>
       <c r="B61" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C61" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-04-01',</v>
-      </c>
-      <c r="D61" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-04-01'</v>
+      </c>
+      <c r="D61">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E61" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-08-01'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-08-01'</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45142,25 +45144,25 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(62,</v>
+      <c r="A62">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>62</v>
       </c>
       <c r="B62" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C62" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-04-08',</v>
-      </c>
-      <c r="D62" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-04-08'</v>
+      </c>
+      <c r="D62">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E62" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2016-02-02'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2016-02-02'</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45168,25 +45170,25 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(63,</v>
+      <c r="A63">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>63</v>
       </c>
       <c r="B63" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C63" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-04-01',</v>
-      </c>
-      <c r="D63" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>15,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-04-01'</v>
+      </c>
+      <c r="D63">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>15</v>
       </c>
       <c r="E63" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2016-03-10'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2016-03-10'</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45195,50 +45197,50 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B64" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C64" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D64" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E64" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G64" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(65,</v>
+      <c r="A65">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>65</v>
       </c>
       <c r="B65" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C65" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-01',</v>
-      </c>
-      <c r="D65" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-01'</v>
+      </c>
+      <c r="D65">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E65" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45246,25 +45248,25 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(66,</v>
+      <c r="A66">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>66</v>
       </c>
       <c r="B66" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C66" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-02',</v>
-      </c>
-      <c r="D66" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-02'</v>
+      </c>
+      <c r="D66">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E66" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45272,51 +45274,51 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(67,</v>
+      <c r="A67">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>67</v>
       </c>
       <c r="B67" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C67" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-03',</v>
-      </c>
-      <c r="D67" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-03'</v>
+      </c>
+      <c r="D67">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E67" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G110" ca="1" si="1">CONCATENATE(A67,B67,C67,D67,E67)</f>
+        <f t="shared" ref="G67:G110" ca="1" si="1">IF(LEN(B67)&gt;0,CONCATENATE("(",A67,",",B67,",",C67,",",D67,",",E67,"),"),"")</f>
         <v>(67,'TUIXYA225410','2016-05-03',5,'2015-05-19'),</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(68,</v>
+      <c r="A68">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>68</v>
       </c>
       <c r="B68" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C68" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-04',</v>
-      </c>
-      <c r="D68" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-04'</v>
+      </c>
+      <c r="D68">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E68" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45324,25 +45326,25 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(69,</v>
+      <c r="A69">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>69</v>
       </c>
       <c r="B69" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C69" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-05',</v>
-      </c>
-      <c r="D69" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-05'</v>
+      </c>
+      <c r="D69">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E69" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45350,25 +45352,25 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(70,</v>
+      <c r="A70">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>70</v>
       </c>
       <c r="B70" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C70" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-06',</v>
-      </c>
-      <c r="D70" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-06'</v>
+      </c>
+      <c r="D70">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E70" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45376,25 +45378,25 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(71,</v>
+      <c r="A71">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>71</v>
       </c>
       <c r="B71" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C71" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-07',</v>
-      </c>
-      <c r="D71" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-07'</v>
+      </c>
+      <c r="D71">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E71" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45402,25 +45404,25 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(72,</v>
+      <c r="A72">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>72</v>
       </c>
       <c r="B72" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C72" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-08',</v>
-      </c>
-      <c r="D72" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>5,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-08'</v>
+      </c>
+      <c r="D72">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>5</v>
       </c>
       <c r="E72" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45429,50 +45431,50 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B73" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C73" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D73" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E73" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G73" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(74,</v>
+      <c r="A74">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>74</v>
       </c>
       <c r="B74" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C74" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-13',</v>
-      </c>
-      <c r="D74" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-13'</v>
+      </c>
+      <c r="D74">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E74" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45480,25 +45482,25 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(75,</v>
+      <c r="A75">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>75</v>
       </c>
       <c r="B75" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C75" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-14',</v>
-      </c>
-      <c r="D75" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-14'</v>
+      </c>
+      <c r="D75">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E75" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45506,25 +45508,25 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(76,</v>
+      <c r="A76">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>76</v>
       </c>
       <c r="B76" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C76" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-18',</v>
-      </c>
-      <c r="D76" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-18'</v>
+      </c>
+      <c r="D76">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E76" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45533,50 +45535,50 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B77" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C77" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D77" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E77" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G77" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(78,</v>
+      <c r="A78">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>78</v>
       </c>
       <c r="B78" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C78" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-19',</v>
-      </c>
-      <c r="D78" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-19'</v>
+      </c>
+      <c r="D78">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E78" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45585,50 +45587,50 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B79" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C79" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D79" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E79" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G79" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(80,</v>
+      <c r="A80">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>80</v>
       </c>
       <c r="B80" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C80" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-20',</v>
-      </c>
-      <c r="D80" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-20'</v>
+      </c>
+      <c r="D80">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E80" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45637,50 +45639,50 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B81" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C81" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D81" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E81" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G81" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(82,</v>
+      <c r="A82">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>82</v>
       </c>
       <c r="B82" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C82" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-21',</v>
-      </c>
-      <c r="D82" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-21'</v>
+      </c>
+      <c r="D82">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E82" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45689,50 +45691,50 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B83" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C83" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D83" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E83" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G83" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(84,</v>
+      <c r="A84">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>84</v>
       </c>
       <c r="B84" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C84" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-22',</v>
-      </c>
-      <c r="D84" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-22'</v>
+      </c>
+      <c r="D84">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E84" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45741,50 +45743,50 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B85" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C85" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D85" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E85" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G85" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(86,</v>
+      <c r="A86">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>86</v>
       </c>
       <c r="B86" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C86" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-23',</v>
-      </c>
-      <c r="D86" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-23'</v>
+      </c>
+      <c r="D86">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E86" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G86" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45793,50 +45795,50 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B87" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C87" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D87" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E87" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G87" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(88,</v>
+      <c r="A88">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>88</v>
       </c>
       <c r="B88" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C88" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-05-26',</v>
-      </c>
-      <c r="D88" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-05-26'</v>
+      </c>
+      <c r="D88">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E88" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45845,50 +45847,50 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B89" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C89" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D89" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E89" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G89" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(90,</v>
+      <c r="A90">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>90</v>
       </c>
       <c r="B90" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C90" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-07-03',</v>
-      </c>
-      <c r="D90" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>27,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-07-03'</v>
+      </c>
+      <c r="D90">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>27</v>
       </c>
       <c r="E90" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45897,76 +45899,76 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B91" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C91" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D91" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E91" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G91" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B92" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C92" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D92" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E92" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G92" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(93,</v>
+      <c r="A93">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>93</v>
       </c>
       <c r="B93" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYZ50502',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYZ50502'</v>
       </c>
       <c r="C93" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D93" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>3,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D93">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>3</v>
       </c>
       <c r="E93" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G93" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -45974,25 +45976,25 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(94,</v>
+      <c r="A94">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>94</v>
       </c>
       <c r="B94" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYZ50502',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYZ50502'</v>
       </c>
       <c r="C94" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D94" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>3,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D94">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>3</v>
       </c>
       <c r="E94" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G94" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -46000,25 +46002,25 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(95,</v>
+      <c r="A95">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>95</v>
       </c>
       <c r="B95" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYZ50502',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYZ50502'</v>
       </c>
       <c r="C95" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-01',</v>
-      </c>
-      <c r="D95" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>3,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-01'</v>
+      </c>
+      <c r="D95">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>3</v>
       </c>
       <c r="E95" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -46027,50 +46029,50 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B96" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C96" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D96" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E96" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G96" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(97,</v>
+      <c r="A97">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>97</v>
       </c>
       <c r="B97" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C97" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-03-01',</v>
-      </c>
-      <c r="D97" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>30,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-03-01'</v>
+      </c>
+      <c r="D97">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>30</v>
       </c>
       <c r="E97" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -46079,102 +46081,102 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B98" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C98" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D98" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E98" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G98" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B99" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C99" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D99" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E99" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G99" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B100" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C100" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D100" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E100" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G100" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(101,</v>
+      <c r="A101">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>101</v>
       </c>
       <c r="B101" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C101" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-03-01',</v>
-      </c>
-      <c r="D101" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>91,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-03-01'</v>
+      </c>
+      <c r="D101">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>91</v>
       </c>
       <c r="E101" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G101" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -46183,232 +46185,232 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B102" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C102" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D102" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E102" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G102" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B103" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C103" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D103" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E103" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G103" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B104" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C104" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D104" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E104" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G104" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B105" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C105" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D105" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E105" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G105" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B106" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C106" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D106" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E106" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G106" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B107" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C107" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D107" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E107" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G107" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B108" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C108" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D108" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E108" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G108" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
         <v/>
       </c>
       <c r="B109" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
         <v/>
       </c>
       <c r="C109" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
         <v/>
       </c>
       <c r="D109" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
         <v/>
       </c>
       <c r="E109" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
         <v/>
       </c>
       <c r="G109" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("(",ROW(),","),"")</f>
-        <v>(110,</v>
+      <c r="A110">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,ROW(),"")</f>
+        <v>110</v>
       </c>
       <c r="B110" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"',"),"")</f>
-        <v>'TUIXYA225410',</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",Tabelle4[[#This Row],[ItemSeq]],"'"),"")</f>
+        <v>'TUIXYA225410'</v>
       </c>
       <c r="C110" s="49" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"',"),"")</f>
-        <v>'2016-01-27',</v>
-      </c>
-      <c r="D110" t="str">
-        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE(Tabelle4[[#This Row],[Duration]],","),"")</f>
-        <v>13,</v>
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,CONCATENATE("'",TEXT(Tabelle4[[#This Row],[ItemStartDate]],"jjjj-MM-tt"),"'"),"")</f>
+        <v>'2016-01-27'</v>
+      </c>
+      <c r="D110">
+        <f>IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,Tabelle4[[#This Row],[Duration]],"")</f>
+        <v>13</v>
       </c>
       <c r="E110" s="49" t="str">
-        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'),"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'),")),"")</f>
-        <v>'2015-05-19'),</v>
+        <f ca="1">IF(LEN(Tabelle4[[#This Row],[ItemStartDate]])&gt;0,IF(Tabelle4[[#This Row],[CurrentDate]]="current date",CONCATENATE("'",TEXT(TODAY(),"jjjj-MM-tt"),"'"),CONCATENATE("'",TEXT(Tabelle4[[#This Row],[CurrentDate]],"jjjj-MM-tt"),"'")),"")</f>
+        <v>'2015-05-19'</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" ca="1" si="1"/>

</xml_diff>